<commit_message>
effect param table 작성 중
</commit_message>
<xml_diff>
--- a/로스트아크/데이터테이블/Effect_Table.xlsx
+++ b/로스트아크/데이터테이블/Effect_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sky20\Desktop\진선\GameDesign\로스트아크\데이터테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F064C4E1-9144-4059-9E7C-BF18E5EAD628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F81184-7DE9-4CB0-9171-60DEE50449D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
+    <workbookView xWindow="9216" yWindow="0" windowWidth="13920" windowHeight="12336" activeTab="1" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="2" r:id="rId1"/>
@@ -1179,7 +1179,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="182">
   <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1340,10 +1340,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>percent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[atk_pwr]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1356,54 +1352,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신의 공격력이 {"atk_pwr"} 증가한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신의 공격력이 {"atk_pwr"}% 증가한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신 및 파티원의 공격력이 {"atk_pwr"} 증가한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신 및 파티원의 공격력이 {"atk_pwr"}% 증가한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"damage"}의 피해를 {"hit_cnt"}번 준다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"damage"}의 고정 피해를 {"hit_cnt"}번 준다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>tick</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TICK 대미지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반 대미지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고정 대미지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최대 체력 비례 대미지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>OBJECT_SPAWN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1412,18 +1364,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"tick_time"}마다 {"damage"}의 피해를 준다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[gauge]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>아이덴티티 게이지를 {"gauge"}만큼 회복한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -1491,30 +1435,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>적에게 주는 피해가 {"damage"}% 증가한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[cooldown]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전체 스킬의 재사용 대기 시간을 {"cooldown"}초 감소시킨다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체 스킬의 재사용 대기 시간을 {"cooldown"}% 감소시킨다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[element]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>스킬에 {"element"}속성을 부여한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cur_hp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1527,10 +1455,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신의 생명력을 {"hp"}만큼 회복한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[max_hp_ratio]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1539,70 +1463,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신 및 파티원의 파티원의 공격력에 자신의 기본 공격력의 {"base_atk_pwr_ratio"}%만큼 더한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[max_hp_ratio,hit_cnt]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대상 최대 체력의 {"max_hp_ratio"}%에 해당하는 피해를 {"hit_cnt"}번 준다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신 및 파티원의 생명력을 {"hp"}만큼 회복한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신의 생명력을 최대 생명력의 {"max_hp_ratio"}%만큼 회복한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신 및 파티원의 생명력을 최대 생명력의 {"max_hp_ratio"}%만큼 회복한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공포에 걸려 행동 불가 상태가 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기절에 걸려 행동 불가 상태가 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>수면에 걸려 행동 불가 상태가 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>감금 상태가 되어 행동 불가 상태가 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>감전에 걸려 행동 불가 상태가 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>동결에 걸려 행동 불가 상태가 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>석화에 걸려 행동 불가 상태가 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지진에 걸려 행동 불가 상태가 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해충에 걸려 행동 불가 상태가 된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>매혹 상태에 빠져 적대적 상태가 되며, 시간이 다 되면 정기가 모두 빠져 사망한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상태이상 - 기절</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1695,14 +1555,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신 및 파티원에게 자신의 최대 생명력의 {"hp_ratio"}%만큼 피해를 흡수하는 보호막을 부여한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신의 최대 생명력의 {"hp_ratio"}%만큼 피해를 흡수하는 보호막을 부여한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>invincibility</t>
   </si>
   <si>
@@ -1725,18 +1577,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>중독 - {"tick_time"}마다 {"damage"}의 피해를 준다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>출혈 - {"tick_time"}마다 {"damage"}의 피해를 준다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>화상 - {"tick_time"}마다 {"damage"}의 [화]속성 마법 피해를 준다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GRANT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1769,30 +1609,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>공격 속성을 [성]속성으로 변환한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격 속성을 [암]속성으로 변환한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격 속성을 [화]속성으로 변환한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격 속성을 [수]속성으로 변환한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격 속성을 [토]속성으로 변환한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격 속성을 [뇌]속성으로 변환한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>projectile</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1805,18 +1621,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>해당 지점에 id = {"obj_id"}인 오브젝트를 생성한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id = {"obj_id"}인 오브젝트를 생성하여 발사한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>id = {"obj_id"}인 소환수를 소환한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>효과가 적용되는 방식</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1829,14 +1633,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>공격력이 {"atk_pwr"}% 감소한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격력이 {"atk_pwr"} 감소한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>방어력 감소</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1861,14 +1657,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>방어력이 {"def"} 감소한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방어력이 {"def"}% 감소한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>outgoing_damage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1881,18 +1669,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>추가 피해가 {"damage"}% 증가한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신 및 파티원의 적에게 주는 피해가 {"damage"}% 증가한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>자신 및 파티원의 추가 피해가 {"damage"}% 증가한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>비율 연산의 기준 스탯</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1905,10 +1681,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>아이덴티티 게이지를 {"gauge"}%만큼 회복한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>피격 이상</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1933,10 +1705,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[dmg,hit_cnt]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>element_fire</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2001,10 +1769,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>자신의 치명타 적중률이 N% 증가한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>weak_point</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2026,10 +1790,6 @@
   </si>
   <si>
     <t>string[]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>효과의 전체 매개 변수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2170,6 +1930,30 @@
   </si>
   <si>
     <t>상태 이상 면역 (파티)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>효과 적용에 필요한 전체 매개 변수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 피해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고정 피해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dot 피해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최대 체력 비례 피해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratio</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2572,7 +2356,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2677,9 +2461,6 @@
     </xf>
     <xf numFmtId="177" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
@@ -3020,8 +2801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF385D5D-99E2-46DF-BA33-B40AE917BBB4}">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
@@ -3039,11 +2820,11 @@
   <sheetData>
     <row r="1" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C3" s="5" t="s">
@@ -3065,13 +2846,13 @@
         <v>0</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="G4" s="8"/>
     </row>
@@ -3090,7 +2871,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>214</v>
+        <v>154</v>
       </c>
       <c r="G5" s="8"/>
     </row>
@@ -3106,7 +2887,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>215</v>
+        <v>155</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -3122,7 +2903,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>216</v>
+        <v>156</v>
       </c>
       <c r="G7" s="8"/>
     </row>
@@ -3138,7 +2919,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>217</v>
+        <v>157</v>
       </c>
       <c r="G8" s="8"/>
     </row>
@@ -3148,13 +2929,13 @@
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="G9" s="8"/>
     </row>
@@ -3164,13 +2945,13 @@
         <v>6</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="G10" s="8"/>
     </row>
@@ -3183,10 +2964,10 @@
         <v>36</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>212</v>
+        <v>153</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>213</v>
+        <v>176</v>
       </c>
       <c r="G11" s="8"/>
     </row>
@@ -3201,7 +2982,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="26" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2"/>
       <c r="F18" s="25"/>
@@ -3409,34 +3190,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC540C7E-1D9A-4204-BA37-262FBD0C3DDD}">
-  <dimension ref="A1:V84"/>
+  <dimension ref="A1:V85"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.8" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.796875" style="36" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.3984375" style="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.3984375" style="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.19921875" style="34" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.296875" style="32" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.09765625" style="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.19921875" style="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="34" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="62.796875" style="35" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.69921875" style="36" customWidth="1"/>
+    <col min="8" max="8" width="14.59765625" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.296875" style="35" customWidth="1"/>
+    <col min="10" max="11" width="15.69921875" style="35" customWidth="1"/>
     <col min="12" max="13" width="15.69921875" style="33" customWidth="1"/>
     <col min="14" max="14" width="18.69921875" style="33" customWidth="1"/>
-    <col min="15" max="18" width="15.69921875" style="36" customWidth="1"/>
+    <col min="15" max="18" width="15.69921875" style="35" customWidth="1"/>
     <col min="19" max="22" width="18.69921875" style="33" customWidth="1"/>
     <col min="23" max="16384" width="8.796875" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>1</v>
@@ -3451,17 +3232,15 @@
         <v>15</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="H1" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="28" t="s">
-        <v>44</v>
-      </c>
+      <c r="I1" s="30"/>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
       <c r="L1" s="2"/>
@@ -3477,8 +3256,8 @@
       <c r="V1" s="2"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A2" s="37" t="s">
-        <v>53</v>
+      <c r="A2" s="36" t="s">
+        <v>177</v>
       </c>
       <c r="B2" s="34">
         <v>1000</v>
@@ -3493,17 +3272,12 @@
         <v>21</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="G2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="I2" s="35" t="s">
-        <v>49</v>
-      </c>
+      <c r="I2" s="31"/>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
       <c r="L2" s="32"/>
@@ -3519,8 +3293,8 @@
       <c r="V2" s="32"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A3" s="37" t="s">
-        <v>54</v>
+      <c r="A3" s="36" t="s">
+        <v>178</v>
       </c>
       <c r="B3" s="34">
         <v>1001</v>
@@ -3535,17 +3309,12 @@
         <v>23</v>
       </c>
       <c r="F3" s="32" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="G3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="I3" s="35" t="s">
-        <v>50</v>
-      </c>
+      <c r="I3" s="31"/>
       <c r="J3" s="31"/>
       <c r="K3" s="31"/>
       <c r="L3" s="32"/>
@@ -3561,8 +3330,8 @@
       <c r="V3" s="32"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A4" s="37" t="s">
-        <v>52</v>
+      <c r="A4" s="36" t="s">
+        <v>179</v>
       </c>
       <c r="B4" s="34">
         <v>1002</v>
@@ -3574,20 +3343,15 @@
         <v>4</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="G4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="I4" s="35" t="s">
-        <v>58</v>
-      </c>
+      <c r="I4" s="31"/>
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
       <c r="L4" s="32"/>
@@ -3603,8 +3367,8 @@
       <c r="V4" s="32"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A5" s="37" t="s">
-        <v>55</v>
+      <c r="A5" s="36" t="s">
+        <v>180</v>
       </c>
       <c r="B5" s="34">
         <v>1003</v>
@@ -3616,20 +3380,15 @@
         <v>4</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>40</v>
+        <v>181</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="I5" s="35" t="s">
-        <v>92</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="I5" s="31"/>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
       <c r="L5" s="32"/>
@@ -3645,6 +3404,7 @@
       <c r="V5" s="32"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="I6" s="31"/>
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
       <c r="L6" s="32"/>
@@ -3659,130 +3419,99 @@
       <c r="U6" s="32"/>
       <c r="V6" s="32"/>
     </row>
-    <row r="7" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="37" t="s">
-        <v>201</v>
-      </c>
-      <c r="B7" s="34">
-        <v>2000</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>45</v>
-      </c>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="I7" s="31"/>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
       <c r="Q7" s="31"/>
       <c r="R7" s="31"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A8" s="37" t="s">
-        <v>220</v>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+    </row>
+    <row r="8" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="36" t="s">
+        <v>143</v>
       </c>
       <c r="B8" s="34">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G8" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H8" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="35" t="s">
-        <v>47</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A9" s="37" t="s">
-        <v>202</v>
+      <c r="A9" s="36" t="s">
+        <v>160</v>
       </c>
       <c r="B9" s="34">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="G9" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="31"/>
-      <c r="P9" s="31"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-    </row>
-    <row r="10" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="37" t="s">
-        <v>221</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A10" s="36" t="s">
+        <v>144</v>
       </c>
       <c r="B10" s="34">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E10" s="32" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="G10" s="32" t="s">
         <v>0</v>
@@ -3790,44 +3519,47 @@
       <c r="H10" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="35" t="s">
-        <v>48</v>
-      </c>
+      <c r="I10" s="31"/>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
       <c r="Q10" s="31"/>
       <c r="R10" s="31"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
     </row>
     <row r="11" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="37" t="s">
-        <v>43</v>
+      <c r="A11" s="36" t="s">
+        <v>161</v>
       </c>
       <c r="B11" s="34">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="C11" s="34" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E11" s="32" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>90</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="I11" s="31"/>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
       <c r="O11" s="31"/>
@@ -3836,33 +3568,31 @@
       <c r="R11" s="31"/>
     </row>
     <row r="12" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="37" t="s">
-        <v>203</v>
+      <c r="A12" s="36" t="s">
+        <v>42</v>
       </c>
       <c r="B12" s="34">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D12" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>175</v>
-      </c>
       <c r="H12" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="I12" s="35" t="s">
-        <v>78</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="I12" s="31"/>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
       <c r="O12" s="31"/>
@@ -3871,33 +3601,31 @@
       <c r="R12" s="31"/>
     </row>
     <row r="13" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="37" t="s">
-        <v>222</v>
+      <c r="A13" s="36" t="s">
+        <v>145</v>
       </c>
       <c r="B13" s="34">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>173</v>
+        <v>120</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="G13" s="32" t="s">
-        <v>175</v>
+        <v>122</v>
       </c>
       <c r="H13" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="I13" s="35" t="s">
-        <v>177</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="I13" s="31"/>
       <c r="J13" s="31"/>
       <c r="K13" s="31"/>
       <c r="O13" s="31"/>
@@ -3906,33 +3634,31 @@
       <c r="R13" s="31"/>
     </row>
     <row r="14" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="37" t="s">
-        <v>204</v>
+      <c r="A14" s="36" t="s">
+        <v>162</v>
       </c>
       <c r="B14" s="34">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="I14" s="35" t="s">
-        <v>176</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="I14" s="31"/>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="O14" s="31"/>
@@ -3941,33 +3667,31 @@
       <c r="R14" s="31"/>
     </row>
     <row r="15" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="37" t="s">
-        <v>223</v>
+      <c r="A15" s="36" t="s">
+        <v>146</v>
       </c>
       <c r="B15" s="34">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>174</v>
+        <v>121</v>
       </c>
       <c r="F15" s="32" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>174</v>
+        <v>121</v>
       </c>
       <c r="H15" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="I15" s="35" t="s">
-        <v>178</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="I15" s="31"/>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
       <c r="O15" s="31"/>
@@ -3976,29 +3700,31 @@
       <c r="R15" s="31"/>
     </row>
     <row r="16" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="37" t="s">
-        <v>200</v>
-      </c>
-      <c r="B16" s="34"/>
+      <c r="A16" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="34">
+        <v>2008</v>
+      </c>
       <c r="C16" s="34" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>205</v>
+        <v>121</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G16" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="H16" s="34"/>
-      <c r="I16" s="35" t="s">
-        <v>206</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="I16" s="31"/>
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="O16" s="31"/>
@@ -4007,12 +3733,27 @@
       <c r="R16" s="31"/>
     </row>
     <row r="17" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="37"/>
+      <c r="A17" s="36" t="s">
+        <v>142</v>
+      </c>
       <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
+      <c r="C17" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>147</v>
+      </c>
       <c r="H17" s="34"/>
-      <c r="I17" s="35"/>
+      <c r="I17" s="31"/>
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
       <c r="O17" s="31"/>
@@ -4020,126 +3761,95 @@
       <c r="Q17" s="31"/>
       <c r="R17" s="31"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="36"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="31"/>
       <c r="J18" s="31"/>
       <c r="K18" s="31"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
       <c r="O18" s="31"/>
       <c r="P18" s="31"/>
       <c r="Q18" s="31"/>
       <c r="R18" s="31"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="32"/>
-    </row>
-    <row r="19" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="B19" s="34">
-        <v>3000</v>
-      </c>
-      <c r="C19" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" s="35" t="s">
-        <v>164</v>
-      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="I19" s="31"/>
       <c r="J19" s="31"/>
       <c r="K19" s="31"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
       <c r="O19" s="31"/>
       <c r="P19" s="31"/>
       <c r="Q19" s="31"/>
       <c r="R19" s="31"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A20" s="37" t="s">
-        <v>167</v>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+    </row>
+    <row r="20" spans="1:22" s="32" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="36" t="s">
+        <v>117</v>
       </c>
       <c r="B20" s="34">
-        <v>3001</v>
+        <v>3000</v>
       </c>
       <c r="C20" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E20" s="32" t="s">
         <v>24</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G20" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H20" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" s="35" t="s">
-        <v>163</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="I20" s="31"/>
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
       <c r="O20" s="31"/>
       <c r="P20" s="31"/>
       <c r="Q20" s="31"/>
       <c r="R20" s="31"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
-      <c r="V20" s="32"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A21" s="37" t="s">
-        <v>165</v>
+      <c r="A21" s="36" t="s">
+        <v>116</v>
       </c>
       <c r="B21" s="34">
-        <v>3002</v>
+        <v>3001</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E21" s="32" t="s">
-        <v>169</v>
+        <v>24</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="G21" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="I21" s="35" t="s">
-        <v>171</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="I21" s="31"/>
       <c r="J21" s="31"/>
       <c r="K21" s="31"/>
       <c r="L21" s="32"/>
@@ -4155,33 +3865,31 @@
       <c r="V21" s="32"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A22" s="37" t="s">
-        <v>166</v>
+      <c r="A22" s="36" t="s">
+        <v>114</v>
       </c>
       <c r="B22" s="34">
-        <v>3003</v>
+        <v>3002</v>
       </c>
       <c r="C22" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E22" s="32" t="s">
-        <v>169</v>
+        <v>118</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G22" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H22" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="I22" s="35" t="s">
-        <v>172</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="I22" s="31"/>
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
       <c r="L22" s="32"/>
@@ -4196,276 +3904,272 @@
       <c r="U22" s="32"/>
       <c r="V22" s="32"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A24" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="B24" s="34">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A23" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B23" s="34">
+        <v>3003</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A25" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" s="34">
         <v>4000</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C25" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="I24" s="35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A25" s="37" t="s">
-        <v>225</v>
-      </c>
-      <c r="B25" s="34">
+      <c r="D25" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A26" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="34">
         <v>4001</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C26" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H25" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="I25" s="35" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A26" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="B26" s="34">
+      <c r="D26" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A27" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27" s="34">
         <v>4002</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C27" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H26" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="I26" s="35" t="s">
+      <c r="D27" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A28" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" s="34">
+        <v>4003</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A29" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="34">
+        <v>4004</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="32" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A27" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="B27" s="34">
-        <v>4003</v>
-      </c>
-      <c r="C27" s="34" t="s">
+      <c r="F29" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A30" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" s="34">
+        <v>4005</v>
+      </c>
+      <c r="C30" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="H27" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="I27" s="35" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A28" s="37" t="s">
-        <v>228</v>
-      </c>
-      <c r="B28" s="34">
-        <v>4004</v>
-      </c>
-      <c r="C28" s="34" t="s">
+      <c r="D30" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A31" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" s="34">
+        <v>4006</v>
+      </c>
+      <c r="C31" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G28" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A29" s="37" t="s">
-        <v>229</v>
-      </c>
-      <c r="B29" s="34">
-        <v>4005</v>
-      </c>
-      <c r="C29" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G29" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H29" s="34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A30" s="37" t="s">
-        <v>230</v>
-      </c>
-      <c r="B30" s="34">
-        <v>4006</v>
-      </c>
-      <c r="C30" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G30" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="H30" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="I30" s="35" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A31" s="37" t="s">
-        <v>231</v>
-      </c>
-      <c r="B31" s="34">
-        <v>4007</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>22</v>
-      </c>
       <c r="D31" s="34" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E31" s="32" t="s">
         <v>7</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="H31" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="I31" s="35" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A32" s="37" t="s">
-        <v>127</v>
+      <c r="A32" s="36" t="s">
+        <v>171</v>
       </c>
       <c r="B32" s="34">
+        <v>4007</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A33" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="34">
         <v>4008</v>
-      </c>
-      <c r="C32" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G32" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H32" s="34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A33" s="37" t="s">
-        <v>128</v>
-      </c>
-      <c r="B33" s="34">
-        <v>4009</v>
       </c>
       <c r="C33" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G33" s="32" t="s">
         <v>0</v>
@@ -4474,157 +4178,154 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A35" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="B35" s="34">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A34" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" s="34">
+        <v>4009</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A36" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="B36" s="34">
         <v>4980</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C36" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="F35" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G35" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35" s="34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A36" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="B36" s="34">
+      <c r="D36" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A37" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B37" s="34">
         <v>4981</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C37" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="F36" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G36" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H36" s="34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="B37" s="34">
+      <c r="D37" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A38" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="B38" s="34">
         <v>4982</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C38" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="F37" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G37" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H37" s="34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="B38" s="34">
+      <c r="D38" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F38" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G38" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A39" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B39" s="34">
         <v>4983</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C39" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E38" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="F38" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G38" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H38" s="34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A40" s="37" t="s">
-        <v>141</v>
-      </c>
-      <c r="B40" s="34">
+      <c r="D39" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F39" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A41" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="34">
         <v>4990</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="F40" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G40" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H40" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="I40" s="35" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A41" s="37" t="s">
-        <v>142</v>
-      </c>
-      <c r="B41" s="34">
-        <v>4991</v>
       </c>
       <c r="C41" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="34" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E41" s="32" t="s">
-        <v>191</v>
+        <v>137</v>
       </c>
       <c r="F41" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G41" s="32" t="s">
         <v>0</v>
@@ -4632,28 +4333,25 @@
       <c r="H41" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I41" s="35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" s="37" t="s">
-        <v>143</v>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A42" s="36" t="s">
+        <v>102</v>
       </c>
       <c r="B42" s="34">
-        <v>4992</v>
+        <v>4991</v>
       </c>
       <c r="C42" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="34" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E42" s="32" t="s">
-        <v>190</v>
+        <v>133</v>
       </c>
       <c r="F42" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G42" s="32" t="s">
         <v>0</v>
@@ -4661,28 +4359,25 @@
       <c r="H42" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I42" s="35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A43" s="37" t="s">
-        <v>144</v>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A43" s="36" t="s">
+        <v>103</v>
       </c>
       <c r="B43" s="34">
-        <v>4993</v>
+        <v>4992</v>
       </c>
       <c r="C43" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E43" s="32" t="s">
-        <v>192</v>
+        <v>132</v>
       </c>
       <c r="F43" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G43" s="32" t="s">
         <v>0</v>
@@ -4690,28 +4385,25 @@
       <c r="H43" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I43" s="35" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A44" s="37" t="s">
-        <v>145</v>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A44" s="36" t="s">
+        <v>104</v>
       </c>
       <c r="B44" s="34">
-        <v>4994</v>
+        <v>4993</v>
       </c>
       <c r="C44" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D44" s="34" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E44" s="32" t="s">
-        <v>193</v>
+        <v>134</v>
       </c>
       <c r="F44" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G44" s="32" t="s">
         <v>0</v>
@@ -4719,28 +4411,25 @@
       <c r="H44" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I44" s="35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A45" s="37" t="s">
-        <v>146</v>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A45" s="36" t="s">
+        <v>105</v>
       </c>
       <c r="B45" s="34">
-        <v>4995</v>
+        <v>4994</v>
       </c>
       <c r="C45" s="34" t="s">
         <v>19</v>
       </c>
       <c r="D45" s="34" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>194</v>
+        <v>135</v>
       </c>
       <c r="F45" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G45" s="32" t="s">
         <v>0</v>
@@ -4748,144 +4437,129 @@
       <c r="H45" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I45" s="35" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A47" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="B47" s="34">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A46" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="34">
+        <v>4995</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G46" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A48" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="34">
         <v>5000</v>
-      </c>
-      <c r="C47" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="E47" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="F47" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="G47" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H47" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="I47" s="35" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A48" s="37" t="s">
-        <v>125</v>
-      </c>
-      <c r="B48" s="34">
-        <v>5001</v>
       </c>
       <c r="C48" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>162</v>
+        <v>91</v>
       </c>
       <c r="F48" s="32" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="G48" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H48" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="I48" s="35" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A49" s="37" t="s">
-        <v>5</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A49" s="36" t="s">
+        <v>90</v>
       </c>
       <c r="B49" s="34">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="C49" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D49" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="F49" s="32" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="G49" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H49" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="I49" s="35" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A50" s="37" t="s">
-        <v>6</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A50" s="36" t="s">
+        <v>5</v>
       </c>
       <c r="B50" s="34">
-        <v>5100</v>
+        <v>5002</v>
       </c>
       <c r="C50" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E50" s="32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F50" s="32" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
       <c r="G50" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="H50" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="I50" s="35" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A51" s="37" t="s">
-        <v>106</v>
+      <c r="H50" s="34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A51" s="36" t="s">
+        <v>6</v>
       </c>
       <c r="B51" s="34">
-        <v>5101</v>
+        <v>5100</v>
       </c>
       <c r="C51" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D51" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="F51" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G51" s="32" t="s">
         <v>0</v>
@@ -4893,28 +4567,25 @@
       <c r="H51" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I51" s="35" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A52" s="37" t="s">
-        <v>107</v>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A52" s="36" t="s">
+        <v>71</v>
       </c>
       <c r="B52" s="34">
-        <v>5102</v>
+        <v>5101</v>
       </c>
       <c r="C52" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D52" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="F52" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G52" s="32" t="s">
         <v>0</v>
@@ -4922,28 +4593,25 @@
       <c r="H52" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I52" s="35" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A53" s="37" t="s">
-        <v>108</v>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A53" s="36" t="s">
+        <v>72</v>
       </c>
       <c r="B53" s="34">
-        <v>5103</v>
+        <v>5102</v>
       </c>
       <c r="C53" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E53" s="32" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="F53" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G53" s="32" t="s">
         <v>0</v>
@@ -4951,28 +4619,25 @@
       <c r="H53" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I53" s="35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A54" s="37" t="s">
-        <v>109</v>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A54" s="36" t="s">
+        <v>73</v>
       </c>
       <c r="B54" s="34">
-        <v>5104</v>
+        <v>5103</v>
       </c>
       <c r="C54" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D54" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="F54" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G54" s="32" t="s">
         <v>0</v>
@@ -4980,28 +4645,25 @@
       <c r="H54" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I54" s="35" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A55" s="37" t="s">
-        <v>110</v>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A55" s="36" t="s">
+        <v>74</v>
       </c>
       <c r="B55" s="34">
-        <v>5105</v>
+        <v>5104</v>
       </c>
       <c r="C55" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="F55" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G55" s="32" t="s">
         <v>0</v>
@@ -5009,28 +4671,25 @@
       <c r="H55" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I55" s="35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A56" s="37" t="s">
-        <v>111</v>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A56" s="36" t="s">
+        <v>75</v>
       </c>
       <c r="B56" s="34">
-        <v>5106</v>
+        <v>5105</v>
       </c>
       <c r="C56" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="F56" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G56" s="32" t="s">
         <v>0</v>
@@ -5038,28 +4697,25 @@
       <c r="H56" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I56" s="35" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A57" s="37" t="s">
-        <v>112</v>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A57" s="36" t="s">
+        <v>76</v>
       </c>
       <c r="B57" s="34">
-        <v>5107</v>
+        <v>5106</v>
       </c>
       <c r="C57" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D57" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E57" s="32" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="F57" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G57" s="32" t="s">
         <v>0</v>
@@ -5067,28 +4723,25 @@
       <c r="H57" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I57" s="35" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A58" s="37" t="s">
-        <v>113</v>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A58" s="36" t="s">
+        <v>77</v>
       </c>
       <c r="B58" s="34">
-        <v>5108</v>
+        <v>5107</v>
       </c>
       <c r="C58" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D58" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E58" s="32" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="F58" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G58" s="32" t="s">
         <v>0</v>
@@ -5096,28 +4749,25 @@
       <c r="H58" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I58" s="35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A59" s="37" t="s">
-        <v>114</v>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A59" s="36" t="s">
+        <v>78</v>
       </c>
       <c r="B59" s="34">
-        <v>5109</v>
+        <v>5108</v>
       </c>
       <c r="C59" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D59" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E59" s="32" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="F59" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G59" s="32" t="s">
         <v>0</v>
@@ -5125,106 +4775,94 @@
       <c r="H59" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I59" s="35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A61" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="B61" s="34">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A60" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" s="34">
+        <v>5109</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E60" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="F60" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G60" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H60" s="32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A62" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" s="34">
         <v>5500</v>
-      </c>
-      <c r="C61" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="D61" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="E61" s="32" t="s">
-        <v>186</v>
-      </c>
-      <c r="F61" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G61" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H61" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="I61" s="35" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A62" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="B62" s="34">
-        <v>5501</v>
       </c>
       <c r="C62" s="34" t="s">
         <v>18</v>
       </c>
       <c r="D62" s="34" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E62" s="32" t="s">
-        <v>184</v>
+        <v>129</v>
       </c>
       <c r="F62" s="32" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="G62" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H62" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="I62" s="35" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="H63" s="32"/>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A65" s="37" t="s">
-        <v>218</v>
-      </c>
-      <c r="B65" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A63" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="34">
+        <v>5501</v>
+      </c>
+      <c r="C63" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F63" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G63" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H63" s="34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="H64" s="32"/>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A66" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B66" s="34">
         <v>6000</v>
-      </c>
-      <c r="C65" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D65" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="F65" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G65" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H65" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="I65" s="35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A66" s="37" t="s">
-        <v>219</v>
-      </c>
-      <c r="B66" s="34">
-        <v>6001</v>
       </c>
       <c r="C66" s="34" t="s">
         <v>19</v>
@@ -5233,27 +4871,24 @@
         <v>34</v>
       </c>
       <c r="E66" s="32" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="F66" s="32" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="G66" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H66" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="I66" s="35" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A67" s="37" t="s">
-        <v>20</v>
+      <c r="A67" s="36" t="s">
+        <v>159</v>
       </c>
       <c r="B67" s="34">
-        <v>6002</v>
+        <v>6001</v>
       </c>
       <c r="C67" s="34" t="s">
         <v>19</v>
@@ -5262,66 +4897,50 @@
         <v>34</v>
       </c>
       <c r="E67" s="32" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="F67" s="32" t="s">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="G67" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H67" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="I67" s="35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A69" s="37" t="s">
-        <v>196</v>
-      </c>
-      <c r="B69" s="34">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A68" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" s="34">
+        <v>6002</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D68" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F68" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G68" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H68" s="34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A70" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="34">
         <v>6500</v>
-      </c>
-      <c r="C69" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D69" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="E69" s="32" t="s">
-        <v>207</v>
-      </c>
-      <c r="F69" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="G69" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H69" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="J69" s="31"/>
-      <c r="K69" s="31"/>
-      <c r="L69" s="32"/>
-      <c r="M69" s="32"/>
-      <c r="N69" s="32"/>
-      <c r="O69" s="31"/>
-      <c r="P69" s="31"/>
-      <c r="Q69" s="31"/>
-      <c r="R69" s="31"/>
-      <c r="S69" s="32"/>
-      <c r="T69" s="32"/>
-      <c r="U69" s="32"/>
-      <c r="V69" s="32"/>
-    </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A70" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="B70" s="34">
-        <v>6501</v>
       </c>
       <c r="C70" s="34" t="s">
         <v>19</v>
@@ -5330,17 +4949,18 @@
         <v>34</v>
       </c>
       <c r="E70" s="32" t="s">
-        <v>208</v>
+        <v>148</v>
       </c>
       <c r="F70" s="32" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G70" s="32" t="s">
         <v>0</v>
       </c>
       <c r="H70" s="34" t="s">
-        <v>210</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="I70" s="31"/>
       <c r="J70" s="31"/>
       <c r="K70" s="31"/>
       <c r="L70" s="32"/>
@@ -5355,38 +4975,52 @@
       <c r="U70" s="32"/>
       <c r="V70" s="32"/>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A72" s="37" t="s">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A71" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B71" s="34">
+        <v>6501</v>
+      </c>
+      <c r="C71" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D71" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="F71" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="G71" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H71" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="I71" s="31"/>
+      <c r="J71" s="31"/>
+      <c r="K71" s="31"/>
+      <c r="L71" s="32"/>
+      <c r="M71" s="32"/>
+      <c r="N71" s="32"/>
+      <c r="O71" s="31"/>
+      <c r="P71" s="31"/>
+      <c r="Q71" s="31"/>
+      <c r="R71" s="31"/>
+      <c r="S71" s="32"/>
+      <c r="T71" s="32"/>
+      <c r="U71" s="32"/>
+      <c r="V71" s="32"/>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A73" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B72" s="34">
+      <c r="B73" s="34">
         <v>7000</v>
-      </c>
-      <c r="C72" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D72" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E72" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F72" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="H72" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="I72" s="35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A73" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="B73" s="34">
-        <v>7001</v>
       </c>
       <c r="C73" s="34" t="s">
         <v>19</v>
@@ -5398,21 +5032,15 @@
         <v>27</v>
       </c>
       <c r="F73" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="G73" s="32" t="s">
-        <v>181</v>
+        <v>57</v>
       </c>
       <c r="H73" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="I73" s="35" t="s">
-        <v>182</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A74" s="37" t="s">
-        <v>29</v>
+      <c r="A74" s="36" t="s">
+        <v>124</v>
       </c>
       <c r="B74" s="34">
         <v>7001</v>
@@ -5424,38 +5052,44 @@
         <v>35</v>
       </c>
       <c r="E74" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F74" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G74" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="H74" s="34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A75" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" s="34">
+        <v>7001</v>
+      </c>
+      <c r="C75" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E75" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F74" s="32" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A76" s="37" t="s">
+      <c r="F75" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A77" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B76" s="34">
+      <c r="B77" s="34">
         <v>7500</v>
-      </c>
-      <c r="C76" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D76" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="E76" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F76" s="32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A77" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B77" s="34">
-        <v>7501</v>
       </c>
       <c r="C77" s="34" t="s">
         <v>19</v>
@@ -5464,103 +5098,135 @@
         <v>35</v>
       </c>
       <c r="E77" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F77" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G77" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H77" s="34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A78" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78" s="34">
+        <v>7501</v>
+      </c>
+      <c r="C78" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E78" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="F77" s="32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A79" s="37" t="s">
+      <c r="F78" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G78" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H78" s="34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="A80" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B79" s="34">
+      <c r="B80" s="34">
         <v>8000</v>
-      </c>
-      <c r="C79" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D79" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="E79" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="F79" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="H79" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="I79" s="35" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A80" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="B80" s="34">
-        <v>8001</v>
       </c>
       <c r="C80" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D80" s="34" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E80" s="32" t="s">
-        <v>155</v>
+        <v>108</v>
       </c>
       <c r="F80" s="32" t="s">
-        <v>161</v>
+        <v>112</v>
+      </c>
+      <c r="G80" s="32" t="s">
+        <v>0</v>
       </c>
       <c r="H80" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="I80" s="35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A81" s="37" t="s">
-        <v>38</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A81" s="36" t="s">
+        <v>54</v>
       </c>
       <c r="B81" s="34">
-        <v>8002</v>
+        <v>8001</v>
       </c>
       <c r="C81" s="34" t="s">
         <v>39</v>
       </c>
       <c r="D81" s="34" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="E81" s="32" t="s">
-        <v>156</v>
+        <v>109</v>
       </c>
       <c r="F81" s="32" t="s">
-        <v>161</v>
+        <v>112</v>
+      </c>
+      <c r="G81" s="32" t="s">
+        <v>0</v>
       </c>
       <c r="H81" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="I81" s="35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A83" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="B83" s="34">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A82" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" s="34">
+        <v>8002</v>
+      </c>
+      <c r="C82" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D82" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E82" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F82" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="G82" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="H82" s="34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A84" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B84" s="34">
         <v>9000</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A84" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="B84" s="34">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A85" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B85" s="34">
         <v>9001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
effect table 하는 중
</commit_message>
<xml_diff>
--- a/로스트아크/데이터테이블/Effect_Table.xlsx
+++ b/로스트아크/데이터테이블/Effect_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sky20\Desktop\진선\GameDesign\로스트아크\데이터테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEC9AFE-393F-4D62-AADE-7AE86F110D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8751881E-010B-4023-B7CD-C436528655EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
+    <workbookView xWindow="-108" yWindow="0" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="2" r:id="rId1"/>
@@ -36,8 +36,167 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>홍진선</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{8DE77F51-34DD-4EC2-80C4-37C3B42042DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[효과의 유형]
+0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>: 피해형</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>: 능력치 증가</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+2</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>: 능력치 감소</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+3</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>: 특수 기능-버프</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+4</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>: 특수 기능-디버프</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+5</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">: 제어
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="104">
   <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -89,24 +248,6 @@
     <t>[ID 넘버링]</t>
   </si>
   <si>
-    <t>1000 ~ 1999 : 피해형</t>
-  </si>
-  <si>
-    <t>2000 ~ 2999 : 능력치 증가</t>
-  </si>
-  <si>
-    <t>3000 ~ 3999 : 능력치 감소</t>
-  </si>
-  <si>
-    <t>4000 ~ 4999 : 특수기능 - 버프</t>
-  </si>
-  <si>
-    <t>5000 ~ 5999 : 특수기능 - 디버프</t>
-  </si>
-  <si>
-    <t>6000 ~ 6999 : 시너지 효과</t>
-  </si>
-  <si>
     <t>효과 ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -119,7 +260,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>category</t>
+    <t>sub_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>효과 세부 유형</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -148,7 +293,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: 피해형(DAMAGE)</t>
+      <t>: 피해형</t>
     </r>
     <r>
       <rPr>
@@ -193,7 +338,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: 능력치 조절(ABILITY)</t>
+      <t>: 능력치 증가</t>
     </r>
     <r>
       <rPr>
@@ -227,7 +372,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: 특수 기능(SPECIAL) </t>
+      <t>: 능력치 감소</t>
     </r>
     <r>
       <rPr>
@@ -238,7 +383,75 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>/</t>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 특수 기능-버프 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">/ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 특수 기능-디버프</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /</t>
     </r>
     <r>
       <rPr>
@@ -261,7 +474,7 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>3</t>
+      <t>5</t>
     </r>
     <r>
       <rPr>
@@ -272,124 +485,348 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>: 제어 (CONTROL)</t>
+      <t>: 제어</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sub_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">효과 세부 유형 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">효과 분류   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 해당없음</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> / </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: 버프 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">/ </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 디버프</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10 ~ 19 : 피해형</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 ~ 199 : 능력치 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200 ~ 299 : 능력치 감소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300 ~ 399 : 특수기능 - 버프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>400 ~ 499 : 특수기능 - 디버프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>500 ~ 599 : 제어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 피해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>direct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>효과에 필요한 전체 매개 변수 목록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>param_key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고정 피해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비례 피해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atk_pwr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격력 고정 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격력 비율 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[base_dmg, hit_cnt, hit_interval, stagger, weak_point, identity_gauge_recover]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[base_dmg, hit_cnt, hit_interval]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[value, duration]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[percent, duration]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[base_dmg, source_target, source_stat, percent, hit_cnt, hit_interval]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격력 고정 감소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격력 비율 감소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회복</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보호막</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피격 이상 면역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상태 이상 면역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경직 면역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>push_immune</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>debuff_immune</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[heal, </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[atk_pwr, duration]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>은신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sleep</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imprison</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>electrocution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>freeze</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>petrify</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>earthquake</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fascination</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공포</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기절</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>석화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해충</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매혹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중독</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출혈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>poison</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bleed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>burn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[tick_dmg, tick_time, duration]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[duration]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경직</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피격 이상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paralysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>paralysis_immune</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>push</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이덴티티 게이지 회복</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>identity_gauge_recover</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이덴티티 게이지 % 회복</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페널티 게이지 획득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>penalty_gauge_gain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>속성 부여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무력화 수치 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부위 파괴 레벨 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stagger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weak_point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[gauge_type, gauge_recover]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[gauge_type, percent]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -401,7 +838,7 @@
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -503,6 +940,23 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -772,7 +1226,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -881,6 +1335,12 @@
     <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -890,11 +1350,11 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1218,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF385D5D-99E2-46DF-BA33-B40AE917BBB4}">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:F9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
@@ -1237,15 +1697,15 @@
     <col min="10" max="16384" width="8.796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="36" t="s">
+    <row r="1" spans="2:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="38"/>
-    </row>
-    <row r="3" spans="2:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="D2" s="39"/>
+      <c r="E2" s="40"/>
+    </row>
+    <row r="3" spans="2:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1260,7 +1720,7 @@
       </c>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
@@ -1275,7 +1735,7 @@
       </c>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -1289,82 +1749,86 @@
       <c r="E5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="39" t="s">
-        <v>19</v>
+      <c r="F5" s="36" t="s">
+        <v>13</v>
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C6" s="16">
         <f t="shared" ref="C6:C11" si="0">ROW(C6)-4</f>
         <v>2</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="40" t="s">
+      <c r="D6" s="17" t="s">
         <v>20</v>
       </c>
+      <c r="E6" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>14</v>
+      </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:12" ht="26.4" x14ac:dyDescent="0.4">
       <c r="C7" s="16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="40" t="s">
-        <v>26</v>
+      <c r="F7" s="37" t="s">
+        <v>18</v>
       </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="2:9" ht="26.4" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C8" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>17</v>
       </c>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C9" s="16">
         <f>ROW(C9)-4</f>
         <v>5</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>30</v>
       </c>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C10" s="16">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="40"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C11" s="16">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1374,90 +1838,100 @@
       <c r="F11" s="19"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="2:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
       <c r="F12" s="23"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="I16" s="2" t="s">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="L15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="F16" s="24"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="A17" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2"/>
       <c r="F17" s="24"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="25" t="s">
-        <v>9</v>
-      </c>
+      <c r="I17" s="3"/>
+      <c r="L17" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C18" s="2"/>
-      <c r="F18" s="24"/>
-      <c r="I18" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F18" s="26"/>
+      <c r="I18" s="3"/>
+      <c r="L18" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C19" s="2"/>
-      <c r="F19" s="26"/>
-      <c r="I19" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F19" s="24"/>
+      <c r="I19" s="3"/>
+      <c r="L19" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C20" s="2"/>
-      <c r="F20" s="24"/>
-      <c r="I20" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F20" s="26"/>
+      <c r="I20" s="3"/>
+      <c r="L20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C21" s="2"/>
-      <c r="F21" s="26"/>
-      <c r="I21" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I21" s="3"/>
+      <c r="L21" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C22" s="2"/>
-      <c r="I22" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="I22" s="3"/>
+      <c r="L22" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C23" s="2"/>
-      <c r="I23" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="F23" s="24"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C24" s="2"/>
-      <c r="F24" s="24"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.4">
@@ -1600,9 +2074,6 @@
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C79" s="2"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.4">
-      <c r="C80" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1615,459 +2086,984 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC540C7E-1D9A-4204-BA37-262FBD0C3DDD}">
-  <dimension ref="A1:V71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC540C7E-1D9A-4204-BA37-262FBD0C3DDD}">
+  <dimension ref="A1:T77"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K20" sqref="B1:K20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.8" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.796875" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.3984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.3984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.19921875" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.296875" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.09765625" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.19921875" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.59765625" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.296875" style="34" customWidth="1"/>
-    <col min="10" max="11" width="15.69921875" style="34" customWidth="1"/>
-    <col min="12" max="13" width="15.69921875" style="32" customWidth="1"/>
-    <col min="14" max="14" width="18.69921875" style="32" customWidth="1"/>
-    <col min="15" max="18" width="15.69921875" style="34" customWidth="1"/>
-    <col min="19" max="22" width="18.69921875" style="32" customWidth="1"/>
-    <col min="23" max="16384" width="8.796875" style="32"/>
+    <col min="3" max="3" width="17.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.59765625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.296875" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.19921875" style="42" customWidth="1"/>
+    <col min="7" max="7" width="5.296875" style="34" customWidth="1"/>
+    <col min="8" max="9" width="15.69921875" style="34" customWidth="1"/>
+    <col min="10" max="11" width="15.69921875" style="32" customWidth="1"/>
+    <col min="12" max="12" width="18.69921875" style="32" customWidth="1"/>
+    <col min="13" max="16" width="15.69921875" style="34" customWidth="1"/>
+    <col min="17" max="20" width="18.69921875" style="32" customWidth="1"/>
+    <col min="21" max="16384" width="8.796875" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="B1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
       <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B2" s="33">
+        <v>10</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="33">
+        <v>0</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
       <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
       <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="30"/>
       <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
       <c r="S2" s="31"/>
       <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B3" s="33">
+        <v>11</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
       <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
       <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="30"/>
       <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
       <c r="S3" s="31"/>
       <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
-      <c r="V3" s="31"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B4" s="33">
+        <v>12</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
       <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="30"/>
       <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
       <c r="S4" s="31"/>
       <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
       <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
       <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
       <c r="S5" s="31"/>
       <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B6" s="33">
+        <v>100</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="33">
+        <v>1</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
       <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
       <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
       <c r="O6" s="30"/>
       <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
       <c r="S6" s="31"/>
       <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B7" s="33">
+        <v>101</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
       <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
       <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
       <c r="O7" s="30"/>
       <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
       <c r="S7" s="31"/>
       <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-    </row>
-    <row r="8" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="35"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
       <c r="O8" s="30"/>
       <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="C9" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="33">
+        <v>1</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="C10" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="33">
+        <v>1</v>
+      </c>
+      <c r="E10" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
       <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
       <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
       <c r="O10" s="30"/>
       <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
       <c r="S10" s="31"/>
       <c r="T10" s="31"/>
-      <c r="U10" s="31"/>
-      <c r="V10" s="31"/>
-    </row>
-    <row r="11" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="35"/>
       <c r="B11" s="33"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
-      <c r="H11" s="33"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="30"/>
       <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
       <c r="O11" s="30"/>
       <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-    </row>
-    <row r="12" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="35"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-    </row>
-    <row r="13" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="35"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="H13" s="33"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B12" s="33">
+        <v>200</v>
+      </c>
+      <c r="C12" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="33">
+        <v>2</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B13" s="33">
+        <v>201</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="33">
+        <v>2</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
       <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
       <c r="O13" s="30"/>
       <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-    </row>
-    <row r="14" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+    </row>
+    <row r="14" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="35"/>
       <c r="B14" s="33"/>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
-      <c r="H14" s="33"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
       <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
       <c r="O14" s="30"/>
       <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-    </row>
-    <row r="15" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="35"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="H15" s="33"/>
+      <c r="B15" s="33">
+        <v>300</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="33">
+        <v>3</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="42"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
       <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
       <c r="O15" s="30"/>
       <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-    </row>
-    <row r="16" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="35"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="H16" s="33"/>
+      <c r="B16" s="33">
+        <v>301</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="33">
+        <v>3</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="42"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
       <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
       <c r="O16" s="30"/>
       <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-    </row>
-    <row r="17" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A17" s="35"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="H17" s="33"/>
+      <c r="B17" s="33">
+        <v>302</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="33">
+        <v>3</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="42"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
       <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
       <c r="O17" s="30"/>
       <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
-    </row>
-    <row r="18" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="35"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="H18" s="33"/>
+      <c r="B18" s="33">
+        <v>303</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="33">
+        <v>3</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
       <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
       <c r="O18" s="30"/>
       <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="35"/>
+      <c r="B19" s="33">
+        <v>304</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="33">
+        <v>3</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="42"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
       <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
       <c r="O19" s="30"/>
       <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="30"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-    </row>
-    <row r="20" spans="1:22" s="31" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="35"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="H20" s="33"/>
+      <c r="B20" s="33">
+        <v>305</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="33">
+        <v>3</v>
+      </c>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
       <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
       <c r="O20" s="30"/>
       <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="35"/>
+      <c r="B21" s="33">
+        <v>306</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="33">
+        <v>3</v>
+      </c>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
       <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="31"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="31"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
       <c r="O21" s="30"/>
       <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="31"/>
-      <c r="V21" s="31"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="35"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
       <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
       <c r="O22" s="30"/>
       <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="I23" s="30"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="31"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
-    </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H41" s="31"/>
-    </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H42" s="31"/>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H43" s="31"/>
-    </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H44" s="31"/>
-    </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H45" s="31"/>
-    </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H46" s="31"/>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H51" s="31"/>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H52" s="31"/>
-    </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H53" s="31"/>
-    </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H54" s="31"/>
-    </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H55" s="31"/>
-    </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H56" s="31"/>
-    </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H57" s="31"/>
-    </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H58" s="31"/>
-    </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H59" s="31"/>
-    </row>
-    <row r="60" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H60" s="31"/>
-    </row>
-    <row r="64" spans="8:8" x14ac:dyDescent="0.4">
-      <c r="H64" s="31"/>
-    </row>
-    <row r="70" spans="9:22" x14ac:dyDescent="0.4">
-      <c r="I70" s="30"/>
-      <c r="J70" s="30"/>
-      <c r="K70" s="30"/>
-      <c r="L70" s="31"/>
-      <c r="M70" s="31"/>
-      <c r="N70" s="31"/>
-      <c r="O70" s="30"/>
-      <c r="P70" s="30"/>
-      <c r="Q70" s="30"/>
-      <c r="R70" s="30"/>
-      <c r="S70" s="31"/>
-      <c r="T70" s="31"/>
-      <c r="U70" s="31"/>
-      <c r="V70" s="31"/>
-    </row>
-    <row r="71" spans="9:22" x14ac:dyDescent="0.4">
-      <c r="I71" s="30"/>
-      <c r="J71" s="30"/>
-      <c r="K71" s="30"/>
-      <c r="L71" s="31"/>
-      <c r="M71" s="31"/>
-      <c r="N71" s="31"/>
-      <c r="O71" s="30"/>
-      <c r="P71" s="30"/>
-      <c r="Q71" s="30"/>
-      <c r="R71" s="30"/>
-      <c r="S71" s="31"/>
-      <c r="T71" s="31"/>
-      <c r="U71" s="31"/>
-      <c r="V71" s="31"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B23" s="33">
+        <v>400</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="33">
+        <v>4</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B24" s="33">
+        <v>401</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="33">
+        <v>4</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="35"/>
+      <c r="B25" s="33">
+        <v>402</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="33">
+        <v>4</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="30"/>
+      <c r="O25" s="30"/>
+      <c r="P25" s="30"/>
+    </row>
+    <row r="26" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="35"/>
+      <c r="B26" s="33">
+        <v>403</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="33">
+        <v>4</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+    </row>
+    <row r="27" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="35"/>
+      <c r="B27" s="33">
+        <v>404</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="33">
+        <v>4</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B28" s="33">
+        <v>405</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="33">
+        <v>4</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="30"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="31"/>
+      <c r="S28" s="31"/>
+      <c r="T28" s="31"/>
+    </row>
+    <row r="29" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="35"/>
+      <c r="B29" s="33">
+        <v>406</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="33">
+        <v>4</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
+      <c r="O29" s="30"/>
+      <c r="P29" s="30"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B30" s="33">
+        <v>407</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="33">
+        <v>4</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="31"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B31" s="33">
+        <v>408</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="33">
+        <v>4</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="31"/>
+      <c r="S31" s="31"/>
+      <c r="T31" s="31"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B32" s="33">
+        <v>409</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="33">
+        <v>4</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="31"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B33" s="33">
+        <v>410</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="33">
+        <v>4</v>
+      </c>
+      <c r="E33" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B34" s="33">
+        <v>411</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="33">
+        <v>4</v>
+      </c>
+      <c r="E34" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B35" s="33">
+        <v>412</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="33">
+        <v>4</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B36" s="33">
+        <v>413</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="33">
+        <v>4</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B37" s="33">
+        <v>414</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="33">
+        <v>4</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B39" s="33">
+        <v>500</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B45" s="33">
+        <v>590</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="33">
+        <v>5</v>
+      </c>
+      <c r="E45" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" s="42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B46" s="33">
+        <v>591</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="33">
+        <v>5</v>
+      </c>
+      <c r="E46" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" s="42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B47" s="33">
+        <v>592</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="33">
+        <v>5</v>
+      </c>
+      <c r="E47" s="42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76" spans="7:20" x14ac:dyDescent="0.4">
+      <c r="G76" s="30"/>
+      <c r="H76" s="30"/>
+      <c r="I76" s="30"/>
+      <c r="J76" s="31"/>
+      <c r="K76" s="31"/>
+      <c r="L76" s="31"/>
+      <c r="M76" s="30"/>
+      <c r="N76" s="30"/>
+      <c r="O76" s="30"/>
+      <c r="P76" s="30"/>
+      <c r="Q76" s="31"/>
+      <c r="R76" s="31"/>
+      <c r="S76" s="31"/>
+      <c r="T76" s="31"/>
+    </row>
+    <row r="77" spans="7:20" x14ac:dyDescent="0.4">
+      <c r="G77" s="30"/>
+      <c r="H77" s="30"/>
+      <c r="I77" s="30"/>
+      <c r="J77" s="31"/>
+      <c r="K77" s="31"/>
+      <c r="L77" s="31"/>
+      <c r="M77" s="30"/>
+      <c r="N77" s="30"/>
+      <c r="O77" s="30"/>
+      <c r="P77" s="30"/>
+      <c r="Q77" s="31"/>
+      <c r="R77" s="31"/>
+      <c r="S77" s="31"/>
+      <c r="T77" s="31"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
effect table - sub_type 수정
</commit_message>
<xml_diff>
--- a/로스트아크/데이터테이블/Effect_Table.xlsx
+++ b/로스트아크/데이터테이블/Effect_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sky20\Desktop\진선\GameDesign\로스트아크\데이터테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCD95A8-3B36-4515-AB2E-CE233FDD5BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8353C4-D0B4-423D-BF7F-8C99FDFB3334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="2" r:id="rId1"/>
@@ -367,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{2C962809-0302-4021-B11A-351686D4935E}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{2C962809-0302-4021-B11A-351686D4935E}">
       <text>
         <r>
           <rPr>
@@ -591,7 +591,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="269">
   <si>
     <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -978,14 +978,6 @@
   </si>
   <si>
     <t>sub_type_value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>type별 상세 효과 유형 key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>type별 상세 효과 유형 value</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2181,6 +2173,71 @@
     <t>40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>sub_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">type별 상세 효과 유형 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(아래의 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[비고 1]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 참고)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[비고 1] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type별 상세 효과</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type = 0 (피해형)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -2190,7 +2247,7 @@
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2332,8 +2389,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2372,12 +2438,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -2603,16 +2675,81 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="0"/>
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
       </top>
       <bottom style="thin">
-        <color theme="0"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2623,10 +2760,27 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -2635,7 +2789,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2747,6 +2901,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="177" fontId="5" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2756,14 +2919,23 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3088,10 +3260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF385D5D-99E2-46DF-BA33-B40AE917BBB4}">
-  <dimension ref="B1:I66"/>
+  <dimension ref="B1:I65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
@@ -3109,11 +3281,11 @@
   <sheetData>
     <row r="1" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="38"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
     </row>
     <row r="3" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C3" s="5" t="s">
@@ -3192,7 +3364,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G7" s="8"/>
     </row>
@@ -3208,69 +3380,68 @@
         <v>2</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.4">
       <c r="C9" s="16">
-        <f>ROW(C9)-4</f>
+        <f t="shared" ref="C9:C10" si="1">ROW(C9)-4</f>
         <v>5</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>95</v>
+        <v>265</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>97</v>
+        <v>266</v>
       </c>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:7" ht="26.4" x14ac:dyDescent="0.4">
       <c r="C10" s="16">
-        <f t="shared" ref="C10:C11" si="1">ROW(C10)-4</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>98</v>
+        <v>253</v>
       </c>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="2:7" ht="26.4" x14ac:dyDescent="0.4">
-      <c r="C11" s="16">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="C15" s="2"/>
+    <row r="11" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="13" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C14" s="43" t="s">
+        <v>267</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="46">
+        <v>1</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>268</v>
+      </c>
+      <c r="E15" s="47"/>
+      <c r="F15" s="48"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.4">
       <c r="C16" s="2"/>
@@ -3422,12 +3593,10 @@
     <row r="65" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C65" s="2"/>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.4">
-      <c r="C66" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3437,10 +3606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC540C7E-1D9A-4204-BA37-262FBD0C3DDD}">
-  <dimension ref="A1:P125"/>
+  <dimension ref="A1:O125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54:F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.8" x14ac:dyDescent="0.4"/>
@@ -3449,17 +3618,17 @@
     <col min="2" max="2" width="6.59765625" style="28" customWidth="1"/>
     <col min="3" max="3" width="25.796875" style="28" customWidth="1"/>
     <col min="4" max="5" width="9.19921875" style="28" customWidth="1"/>
-    <col min="6" max="6" width="14.09765625" style="34" customWidth="1"/>
-    <col min="7" max="7" width="15.59765625" style="34" customWidth="1"/>
-    <col min="8" max="8" width="11.09765625" style="34" customWidth="1"/>
-    <col min="9" max="9" width="5.296875" style="29" customWidth="1"/>
-    <col min="10" max="12" width="15.69921875" style="29" customWidth="1"/>
-    <col min="13" max="16" width="18.69921875" style="27" customWidth="1"/>
-    <col min="17" max="16384" width="8.796875" style="27"/>
+    <col min="6" max="6" width="15.59765625" style="34" customWidth="1"/>
+    <col min="7" max="7" width="11.09765625" style="34" customWidth="1"/>
+    <col min="8" max="8" width="5.296875" style="29" customWidth="1"/>
+    <col min="9" max="9" width="14.09765625" style="34" customWidth="1"/>
+    <col min="10" max="11" width="15.69921875" style="29" customWidth="1"/>
+    <col min="12" max="15" width="18.69921875" style="27" customWidth="1"/>
+    <col min="16" max="16384" width="8.796875" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="37" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="23" t="s">
@@ -3474,26 +3643,25 @@
       <c r="E1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="24"/>
+      <c r="I1" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="24"/>
       <c r="J1" s="24"/>
       <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A2" s="41" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A2" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="28">
@@ -3508,26 +3676,25 @@
       <c r="E2" s="28">
         <v>0</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="25"/>
+      <c r="I2" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2" s="25"/>
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
+      <c r="L2" s="26"/>
       <c r="M2" s="26"/>
       <c r="N2" s="26"/>
       <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A3" s="41" t="s">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A3" s="38" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="28">
@@ -3542,26 +3709,25 @@
       <c r="E3" s="28">
         <v>0</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
+      <c r="L3" s="26"/>
       <c r="M3" s="26"/>
       <c r="N3" s="26"/>
       <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A4" s="41" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A4" s="38" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="28">
@@ -3576,50 +3742,48 @@
       <c r="E4" s="28">
         <v>0</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
+      <c r="L4" s="26"/>
       <c r="M4" s="26"/>
       <c r="N4" s="26"/>
       <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A5" s="41" t="s">
-        <v>212</v>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A5" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="F5" s="28"/>
-      <c r="I5" s="25"/>
+        <v>210</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="28"/>
       <c r="J5" s="25"/>
       <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
+      <c r="L5" s="26"/>
       <c r="M5" s="26"/>
       <c r="N5" s="26"/>
       <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A6" s="41" t="s">
-        <v>139</v>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A6" s="38" t="s">
+        <v>137</v>
       </c>
       <c r="B6" s="28">
         <v>1000</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D6" s="28">
         <v>1</v>
@@ -3627,33 +3791,32 @@
       <c r="E6" s="28">
         <v>1</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" s="25"/>
+      <c r="I6" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="H6" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I6" s="25"/>
       <c r="J6" s="25"/>
       <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
+      <c r="L6" s="26"/>
       <c r="M6" s="26"/>
       <c r="N6" s="26"/>
       <c r="O6" s="26"/>
-      <c r="P6" s="26"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A7" s="41" t="s">
-        <v>140</v>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A7" s="38" t="s">
+        <v>138</v>
       </c>
       <c r="B7" s="28">
         <v>1001</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D7" s="28">
         <v>1</v>
@@ -3661,33 +3824,32 @@
       <c r="E7" s="28">
         <v>1</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" s="25"/>
+      <c r="I7" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="25"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="26"/>
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
       <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A8" s="41" t="s">
-        <v>141</v>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A8" s="38" t="s">
+        <v>139</v>
       </c>
       <c r="B8" s="28">
         <v>1002</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D8" s="28">
         <v>1</v>
@@ -3695,33 +3857,32 @@
       <c r="E8" s="28">
         <v>1</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="25"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="26"/>
       <c r="M8" s="26"/>
       <c r="N8" s="26"/>
       <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A9" s="41" t="s">
-        <v>182</v>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" s="38" t="s">
+        <v>180</v>
       </c>
       <c r="B9" s="28">
         <v>1003</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D9" s="28">
         <v>1</v>
@@ -3729,33 +3890,32 @@
       <c r="E9" s="28">
         <v>1</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="25"/>
+      <c r="I9" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="34" t="s">
-        <v>194</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="25"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="26"/>
       <c r="M9" s="26"/>
       <c r="N9" s="26"/>
       <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A10" s="41" t="s">
-        <v>183</v>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A10" s="38" t="s">
+        <v>181</v>
       </c>
       <c r="B10" s="28">
         <v>1004</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D10" s="28">
         <v>1</v>
@@ -3763,33 +3923,32 @@
       <c r="E10" s="28">
         <v>1</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" s="25"/>
+      <c r="I10" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>195</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="25"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="26"/>
       <c r="M10" s="26"/>
       <c r="N10" s="26"/>
       <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A11" s="41" t="s">
-        <v>185</v>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A11" s="38" t="s">
+        <v>183</v>
       </c>
       <c r="B11" s="28">
         <v>1005</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D11" s="28">
         <v>1</v>
@@ -3797,33 +3956,32 @@
       <c r="E11" s="28">
         <v>1</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="H11" s="25"/>
+      <c r="I11" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G11" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="25"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="26"/>
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A12" s="41" t="s">
-        <v>184</v>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A12" s="38" t="s">
+        <v>182</v>
       </c>
       <c r="B12" s="28">
         <v>1006</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D12" s="28">
         <v>1</v>
@@ -3831,33 +3989,32 @@
       <c r="E12" s="28">
         <v>1</v>
       </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" s="25"/>
+      <c r="I12" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="H12" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="25"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26"/>
       <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A13" s="41" t="s">
-        <v>186</v>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A13" s="38" t="s">
+        <v>184</v>
       </c>
       <c r="B13" s="28">
         <v>1007</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D13" s="28">
         <v>1</v>
@@ -3865,33 +4022,32 @@
       <c r="E13" s="28">
         <v>1</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="34" t="s">
+        <v>196</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="25"/>
+      <c r="I13" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="34" t="s">
-        <v>198</v>
-      </c>
-      <c r="H13" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="25"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="26"/>
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A14" s="41" t="s">
-        <v>187</v>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A14" s="38" t="s">
+        <v>185</v>
       </c>
       <c r="B14" s="28">
         <v>1008</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D14" s="28">
         <v>1</v>
@@ -3899,27 +4055,26 @@
       <c r="E14" s="28">
         <v>1</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="H14" s="25"/>
+      <c r="I14" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="H14" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="25"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="26"/>
       <c r="M14" s="26"/>
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A15" s="41" t="s">
-        <v>138</v>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A15" s="38" t="s">
+        <v>136</v>
       </c>
       <c r="B15" s="28">
         <v>1009</v>
@@ -3933,27 +4088,26 @@
       <c r="E15" s="28">
         <v>1</v>
       </c>
-      <c r="F15" s="28" t="s">
+      <c r="F15" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" s="25"/>
+      <c r="I15" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="25"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="26"/>
       <c r="M15" s="26"/>
       <c r="N15" s="26"/>
       <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A16" s="41" t="s">
-        <v>137</v>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A16" s="38" t="s">
+        <v>135</v>
       </c>
       <c r="B16" s="28">
         <v>1010</v>
@@ -3967,33 +4121,32 @@
       <c r="E16" s="28">
         <v>1</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" s="25"/>
+      <c r="I16" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="I16" s="25"/>
       <c r="J16" s="25"/>
       <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
+      <c r="L16" s="26"/>
       <c r="M16" s="26"/>
       <c r="N16" s="26"/>
       <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A17" s="41" t="s">
-        <v>150</v>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A17" s="38" t="s">
+        <v>148</v>
       </c>
       <c r="B17" s="28">
         <v>1011</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D17" s="28">
         <v>1</v>
@@ -4001,33 +4154,32 @@
       <c r="E17" s="28">
         <v>1</v>
       </c>
-      <c r="F17" s="28" t="s">
+      <c r="F17" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" s="25"/>
+      <c r="I17" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I17" s="25"/>
       <c r="J17" s="25"/>
       <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
+      <c r="L17" s="26"/>
       <c r="M17" s="26"/>
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A18" s="41" t="s">
-        <v>151</v>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A18" s="38" t="s">
+        <v>149</v>
       </c>
       <c r="B18" s="28">
         <v>1012</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D18" s="28">
         <v>1</v>
@@ -4035,33 +4187,32 @@
       <c r="E18" s="28">
         <v>1</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" s="25"/>
+      <c r="I18" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="H18" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="I18" s="25"/>
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
+      <c r="L18" s="26"/>
       <c r="M18" s="26"/>
       <c r="N18" s="26"/>
       <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A19" s="41" t="s">
-        <v>148</v>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A19" s="38" t="s">
+        <v>146</v>
       </c>
       <c r="B19" s="28">
         <v>1013</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D19" s="28">
         <v>1</v>
@@ -4069,33 +4220,32 @@
       <c r="E19" s="28">
         <v>1</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="25"/>
+      <c r="I19" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I19" s="25"/>
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
+      <c r="L19" s="26"/>
       <c r="M19" s="26"/>
       <c r="N19" s="26"/>
       <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A20" s="41" t="s">
-        <v>149</v>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A20" s="38" t="s">
+        <v>147</v>
       </c>
       <c r="B20" s="28">
         <v>1014</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D20" s="28">
         <v>1</v>
@@ -4103,33 +4253,32 @@
       <c r="E20" s="28">
         <v>1</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="H20" s="25"/>
+      <c r="I20" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="H20" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
+      <c r="L20" s="26"/>
       <c r="M20" s="26"/>
       <c r="N20" s="26"/>
       <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A21" s="41" t="s">
-        <v>180</v>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A21" s="38" t="s">
+        <v>178</v>
       </c>
       <c r="B21" s="28">
         <v>1015</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D21" s="28">
         <v>1</v>
@@ -4137,33 +4286,32 @@
       <c r="E21" s="28">
         <v>1</v>
       </c>
-      <c r="F21" s="28" t="s">
+      <c r="F21" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="25"/>
+      <c r="I21" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I21" s="25"/>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
+      <c r="L21" s="26"/>
       <c r="M21" s="26"/>
       <c r="N21" s="26"/>
       <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A22" s="41" t="s">
-        <v>181</v>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A22" s="38" t="s">
+        <v>179</v>
       </c>
       <c r="B22" s="28">
         <v>1016</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D22" s="28">
         <v>1</v>
@@ -4171,33 +4319,32 @@
       <c r="E22" s="28">
         <v>1</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="34" t="s">
+        <v>199</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="H22" s="25"/>
+      <c r="I22" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
+      <c r="L22" s="26"/>
       <c r="M22" s="26"/>
       <c r="N22" s="26"/>
       <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A23" s="41" t="s">
-        <v>174</v>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A23" s="38" t="s">
+        <v>172</v>
       </c>
       <c r="B23" s="28">
         <v>1017</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D23" s="28">
         <v>1</v>
@@ -4205,33 +4352,32 @@
       <c r="E23" s="28">
         <v>1</v>
       </c>
-      <c r="F23" s="28" t="s">
+      <c r="F23" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H23" s="25"/>
+      <c r="I23" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G23" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="H23" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I23" s="25"/>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
+      <c r="L23" s="26"/>
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
       <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A24" s="41" t="s">
-        <v>160</v>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A24" s="38" t="s">
+        <v>158</v>
       </c>
       <c r="B24" s="28">
         <v>1018</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D24" s="28">
         <v>1</v>
@@ -4239,33 +4385,32 @@
       <c r="E24" s="28">
         <v>1</v>
       </c>
-      <c r="F24" s="28" t="s">
+      <c r="F24" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H24" s="25"/>
+      <c r="I24" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I24" s="25"/>
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
+      <c r="L24" s="26"/>
       <c r="M24" s="26"/>
       <c r="N24" s="26"/>
       <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A25" s="41" t="s">
-        <v>161</v>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A25" s="38" t="s">
+        <v>159</v>
       </c>
       <c r="B25" s="28">
         <v>1019</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D25" s="28">
         <v>1</v>
@@ -4273,33 +4418,32 @@
       <c r="E25" s="28">
         <v>1</v>
       </c>
-      <c r="F25" s="28" t="s">
+      <c r="F25" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="H25" s="25"/>
+      <c r="I25" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G25" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="H25" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="I25" s="25"/>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
+      <c r="L25" s="26"/>
       <c r="M25" s="26"/>
       <c r="N25" s="26"/>
       <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A26" s="41" t="s">
-        <v>162</v>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A26" s="38" t="s">
+        <v>160</v>
       </c>
       <c r="B26" s="28">
         <v>1020</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D26" s="28">
         <v>1</v>
@@ -4307,33 +4451,32 @@
       <c r="E26" s="28">
         <v>1</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" s="25"/>
+      <c r="I26" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="H26" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I26" s="25"/>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
+      <c r="L26" s="26"/>
       <c r="M26" s="26"/>
       <c r="N26" s="26"/>
       <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A27" s="41" t="s">
-        <v>163</v>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A27" s="38" t="s">
+        <v>161</v>
       </c>
       <c r="B27" s="28">
         <v>1021</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D27" s="28">
         <v>1</v>
@@ -4341,33 +4484,32 @@
       <c r="E27" s="28">
         <v>1</v>
       </c>
-      <c r="F27" s="28" t="s">
+      <c r="F27" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="25"/>
+      <c r="I27" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G27" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="H27" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="I27" s="25"/>
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
+      <c r="L27" s="26"/>
       <c r="M27" s="26"/>
       <c r="N27" s="26"/>
       <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A28" s="41" t="s">
-        <v>152</v>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A28" s="38" t="s">
+        <v>150</v>
       </c>
       <c r="B28" s="28">
         <v>1022</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D28" s="28">
         <v>1</v>
@@ -4375,33 +4517,32 @@
       <c r="E28" s="28">
         <v>1</v>
       </c>
-      <c r="F28" s="28" t="s">
+      <c r="F28" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H28" s="25"/>
+      <c r="I28" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G28" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="H28" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I28" s="25"/>
       <c r="J28" s="25"/>
       <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
+      <c r="L28" s="26"/>
       <c r="M28" s="26"/>
       <c r="N28" s="26"/>
       <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A29" s="41" t="s">
-        <v>153</v>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A29" s="38" t="s">
+        <v>151</v>
       </c>
       <c r="B29" s="28">
         <v>1023</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D29" s="28">
         <v>1</v>
@@ -4409,33 +4550,32 @@
       <c r="E29" s="28">
         <v>1</v>
       </c>
-      <c r="F29" s="28" t="s">
+      <c r="F29" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H29" s="25"/>
+      <c r="I29" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="H29" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I29" s="25"/>
       <c r="J29" s="25"/>
       <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
+      <c r="L29" s="26"/>
       <c r="M29" s="26"/>
       <c r="N29" s="26"/>
       <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A30" s="41" t="s">
-        <v>154</v>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A30" s="38" t="s">
+        <v>152</v>
       </c>
       <c r="B30" s="28">
         <v>1024</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D30" s="28">
         <v>1</v>
@@ -4443,33 +4583,32 @@
       <c r="E30" s="28">
         <v>1</v>
       </c>
-      <c r="F30" s="28" t="s">
+      <c r="F30" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H30" s="25"/>
+      <c r="I30" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G30" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="H30" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I30" s="25"/>
       <c r="J30" s="25"/>
       <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
+      <c r="L30" s="26"/>
       <c r="M30" s="26"/>
       <c r="N30" s="26"/>
       <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A31" s="41" t="s">
-        <v>155</v>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A31" s="38" t="s">
+        <v>153</v>
       </c>
       <c r="B31" s="28">
         <v>1025</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D31" s="28">
         <v>1</v>
@@ -4477,33 +4616,32 @@
       <c r="E31" s="28">
         <v>1</v>
       </c>
-      <c r="F31" s="28" t="s">
+      <c r="F31" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31" s="25"/>
+      <c r="I31" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="H31" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I31" s="25"/>
       <c r="J31" s="25"/>
       <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
+      <c r="L31" s="26"/>
       <c r="M31" s="26"/>
       <c r="N31" s="26"/>
       <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A32" s="41" t="s">
-        <v>216</v>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A32" s="38" t="s">
+        <v>214</v>
       </c>
       <c r="B32" s="28">
         <v>1026</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D32" s="28">
         <v>1</v>
@@ -4511,33 +4649,32 @@
       <c r="E32" s="28">
         <v>1</v>
       </c>
-      <c r="F32" s="28" t="s">
+      <c r="F32" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H32" s="25"/>
+      <c r="I32" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="34" t="s">
-        <v>218</v>
-      </c>
-      <c r="H32" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I32" s="25"/>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
+      <c r="L32" s="26"/>
       <c r="M32" s="26"/>
       <c r="N32" s="26"/>
       <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A33" s="41" t="s">
-        <v>156</v>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A33" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="B33" s="28">
         <v>1027</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D33" s="28">
         <v>1</v>
@@ -4545,33 +4682,32 @@
       <c r="E33" s="28">
         <v>1</v>
       </c>
-      <c r="F33" s="28" t="s">
+      <c r="F33" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H33" s="25"/>
+      <c r="I33" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="H33" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I33" s="25"/>
-      <c r="J33" s="27"/>
+      <c r="J33" s="25"/>
       <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
+      <c r="L33" s="26"/>
       <c r="M33" s="26"/>
       <c r="N33" s="26"/>
       <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A34" s="41" t="s">
-        <v>157</v>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A34" s="38" t="s">
+        <v>155</v>
       </c>
       <c r="B34" s="28">
         <v>1028</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D34" s="28">
         <v>1</v>
@@ -4579,50 +4715,48 @@
       <c r="E34" s="28">
         <v>1</v>
       </c>
-      <c r="F34" s="28" t="s">
+      <c r="F34" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="H34" s="25"/>
+      <c r="I34" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G34" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="H34" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="25"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="26"/>
       <c r="M34" s="26"/>
       <c r="N34" s="26"/>
       <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A35" s="41" t="s">
-        <v>212</v>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A35" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="F35" s="28"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="25"/>
+        <v>210</v>
+      </c>
+      <c r="H35" s="25"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="26"/>
       <c r="M35" s="26"/>
       <c r="N35" s="26"/>
       <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
-    </row>
-    <row r="36" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="41" t="s">
+    </row>
+    <row r="36" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="38" t="s">
         <v>65</v>
       </c>
       <c r="B36" s="28">
         <v>1990</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D36" s="28">
         <v>0</v>
@@ -4630,29 +4764,28 @@
       <c r="E36" s="28">
         <v>1</v>
       </c>
-      <c r="F36" s="28" t="s">
+      <c r="F36" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="26">
+        <v>10</v>
+      </c>
+      <c r="H36" s="25"/>
+      <c r="I36" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G36" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="H36" s="26">
-        <v>10</v>
-      </c>
-      <c r="I36" s="25"/>
       <c r="J36" s="25"/>
       <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-    </row>
-    <row r="37" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="41" t="s">
+    </row>
+    <row r="37" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="38" t="s">
         <v>66</v>
       </c>
       <c r="B37" s="28">
         <v>1991</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D37" s="28">
         <v>0</v>
@@ -4660,46 +4793,44 @@
       <c r="E37" s="28">
         <v>1</v>
       </c>
-      <c r="F37" s="28" t="s">
+      <c r="F37" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G37" s="26">
+        <v>10</v>
+      </c>
+      <c r="H37" s="25"/>
+      <c r="I37" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G37" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" s="26">
-        <v>10</v>
-      </c>
-      <c r="I37" s="25"/>
       <c r="J37" s="25"/>
       <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A38" s="41" t="s">
-        <v>212</v>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A38" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="F38" s="28"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="25"/>
+        <v>210</v>
+      </c>
+      <c r="H38" s="25"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="26"/>
       <c r="M38" s="26"/>
       <c r="N38" s="26"/>
       <c r="O38" s="26"/>
-      <c r="P38" s="26"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A39" s="41" t="s">
-        <v>213</v>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A39" s="38" t="s">
+        <v>211</v>
       </c>
       <c r="B39" s="28">
         <v>2000</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D39" s="28">
         <v>2</v>
@@ -4707,25 +4838,25 @@
       <c r="E39" s="28">
         <v>1</v>
       </c>
-      <c r="F39" s="28" t="s">
+      <c r="F39" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="I39" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G39" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="H39" s="34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A40" s="41" t="s">
-        <v>214</v>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A40" s="38" t="s">
+        <v>212</v>
       </c>
       <c r="B40" s="28">
         <v>2001</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D40" s="28">
         <v>2</v>
@@ -4733,33 +4864,32 @@
       <c r="E40" s="28">
         <v>1</v>
       </c>
-      <c r="F40" s="28" t="s">
+      <c r="F40" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="H40" s="25"/>
+      <c r="I40" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G40" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="H40" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="I40" s="25"/>
       <c r="J40" s="25"/>
       <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
+      <c r="L40" s="26"/>
       <c r="M40" s="26"/>
       <c r="N40" s="26"/>
       <c r="O40" s="26"/>
-      <c r="P40" s="26"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A41" s="41" t="s">
-        <v>221</v>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A41" s="38" t="s">
+        <v>219</v>
       </c>
       <c r="B41" s="28">
         <v>2002</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D41" s="28">
         <v>2</v>
@@ -4767,33 +4897,32 @@
       <c r="E41" s="28">
         <v>1</v>
       </c>
-      <c r="F41" s="28" t="s">
+      <c r="F41" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="G41" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="H41" s="25"/>
+      <c r="I41" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G41" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="H41" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="I41" s="25"/>
       <c r="J41" s="25"/>
       <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
+      <c r="L41" s="26"/>
       <c r="M41" s="26"/>
       <c r="N41" s="26"/>
       <c r="O41" s="26"/>
-      <c r="P41" s="26"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A42" s="41" t="s">
-        <v>223</v>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A42" s="38" t="s">
+        <v>221</v>
       </c>
       <c r="B42" s="28">
         <v>2003</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D42" s="28">
         <v>2</v>
@@ -4801,33 +4930,32 @@
       <c r="E42" s="28">
         <v>1</v>
       </c>
-      <c r="F42" s="28" t="s">
+      <c r="F42" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="G42" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="H42" s="25"/>
+      <c r="I42" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G42" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="H42" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="I42" s="25"/>
       <c r="J42" s="25"/>
       <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
+      <c r="L42" s="26"/>
       <c r="M42" s="26"/>
       <c r="N42" s="26"/>
       <c r="O42" s="26"/>
-      <c r="P42" s="26"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A43" s="41" t="s">
-        <v>225</v>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A43" s="38" t="s">
+        <v>223</v>
       </c>
       <c r="B43" s="28">
         <v>2004</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D43" s="28">
         <v>2</v>
@@ -4835,33 +4963,32 @@
       <c r="E43" s="28">
         <v>1</v>
       </c>
-      <c r="F43" s="28" t="s">
+      <c r="F43" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="G43" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="H43" s="25"/>
+      <c r="I43" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G43" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="H43" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="I43" s="25"/>
       <c r="J43" s="25"/>
       <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
+      <c r="L43" s="26"/>
       <c r="M43" s="26"/>
       <c r="N43" s="26"/>
       <c r="O43" s="26"/>
-      <c r="P43" s="26"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A44" s="41" t="s">
-        <v>226</v>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A44" s="38" t="s">
+        <v>224</v>
       </c>
       <c r="B44" s="28">
         <v>2005</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D44" s="28">
         <v>2</v>
@@ -4869,33 +4996,32 @@
       <c r="E44" s="28">
         <v>1</v>
       </c>
-      <c r="F44" s="28" t="s">
+      <c r="F44" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="G44" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="H44" s="25"/>
+      <c r="I44" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G44" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="H44" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="I44" s="25"/>
       <c r="J44" s="25"/>
       <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
+      <c r="L44" s="26"/>
       <c r="M44" s="26"/>
       <c r="N44" s="26"/>
       <c r="O44" s="26"/>
-      <c r="P44" s="26"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A45" s="41" t="s">
-        <v>219</v>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A45" s="38" t="s">
+        <v>217</v>
       </c>
       <c r="B45" s="28">
         <v>2006</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D45" s="28">
         <v>2</v>
@@ -4903,33 +5029,32 @@
       <c r="E45" s="28">
         <v>1</v>
       </c>
-      <c r="F45" s="28" t="s">
+      <c r="F45" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="G45" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="H45" s="25"/>
+      <c r="I45" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G45" s="34" t="s">
-        <v>218</v>
-      </c>
-      <c r="H45" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="I45" s="25"/>
       <c r="J45" s="25"/>
       <c r="K45" s="25"/>
-      <c r="L45" s="25"/>
+      <c r="L45" s="26"/>
       <c r="M45" s="26"/>
       <c r="N45" s="26"/>
       <c r="O45" s="26"/>
-      <c r="P45" s="26"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A46" s="41" t="s">
-        <v>215</v>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A46" s="38" t="s">
+        <v>213</v>
       </c>
       <c r="B46" s="28">
         <v>2007</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D46" s="28">
         <v>2</v>
@@ -4937,33 +5062,32 @@
       <c r="E46" s="28">
         <v>1</v>
       </c>
-      <c r="F46" s="28" t="s">
+      <c r="F46" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="G46" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="H46" s="25"/>
+      <c r="I46" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G46" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="H46" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="I46" s="25"/>
       <c r="J46" s="25"/>
       <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
+      <c r="L46" s="26"/>
       <c r="M46" s="26"/>
       <c r="N46" s="26"/>
       <c r="O46" s="26"/>
-      <c r="P46" s="26"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A47" s="41" t="s">
-        <v>220</v>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A47" s="38" t="s">
+        <v>218</v>
       </c>
       <c r="B47" s="28">
         <v>2008</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D47" s="28">
         <v>2</v>
@@ -4971,50 +5095,48 @@
       <c r="E47" s="28">
         <v>1</v>
       </c>
-      <c r="F47" s="28" t="s">
+      <c r="F47" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="G47" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="H47" s="25"/>
+      <c r="I47" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G47" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="H47" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="I47" s="25"/>
       <c r="J47" s="25"/>
       <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
+      <c r="L47" s="26"/>
       <c r="M47" s="26"/>
       <c r="N47" s="26"/>
       <c r="O47" s="26"/>
-      <c r="P47" s="26"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A48" s="41" t="s">
-        <v>212</v>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A48" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="F48" s="28"/>
-      <c r="I48" s="25"/>
+        <v>210</v>
+      </c>
+      <c r="H48" s="25"/>
+      <c r="I48" s="28"/>
       <c r="J48" s="25"/>
       <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
+      <c r="L48" s="26"/>
       <c r="M48" s="26"/>
       <c r="N48" s="26"/>
       <c r="O48" s="26"/>
-      <c r="P48" s="26"/>
-    </row>
-    <row r="49" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="42" t="s">
+    </row>
+    <row r="49" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B49" s="28">
         <v>2990</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D49" s="28">
         <v>0</v>
@@ -5022,46 +5144,44 @@
       <c r="E49" s="28">
         <v>1</v>
       </c>
-      <c r="F49" s="28" t="s">
+      <c r="F49" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="G49" s="26">
+        <v>10</v>
+      </c>
+      <c r="H49" s="25"/>
+      <c r="I49" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="G49" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="H49" s="26">
-        <v>10</v>
-      </c>
-      <c r="I49" s="25"/>
       <c r="J49" s="25"/>
       <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A50" s="41" t="s">
-        <v>212</v>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A50" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="F50" s="28"/>
-      <c r="I50" s="25"/>
+        <v>210</v>
+      </c>
+      <c r="H50" s="25"/>
+      <c r="I50" s="28"/>
       <c r="J50" s="25"/>
       <c r="K50" s="25"/>
-      <c r="L50" s="25"/>
+      <c r="L50" s="26"/>
       <c r="M50" s="26"/>
       <c r="N50" s="26"/>
       <c r="O50" s="26"/>
-      <c r="P50" s="26"/>
-    </row>
-    <row r="51" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="41" t="s">
+    </row>
+    <row r="51" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="38" t="s">
         <v>29</v>
       </c>
       <c r="B51" s="28">
         <v>3000</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D51" s="28">
         <v>1</v>
@@ -5070,28 +5190,27 @@
         <v>2</v>
       </c>
       <c r="F51" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="G51" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H51" s="25"/>
+      <c r="I51" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="G51" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="H51" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I51" s="25"/>
       <c r="J51" s="25"/>
       <c r="K51" s="25"/>
-      <c r="L51" s="25"/>
-    </row>
-    <row r="52" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="41" t="s">
+    </row>
+    <row r="52" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="38" t="s">
         <v>27</v>
       </c>
       <c r="B52" s="28">
         <v>3001</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D52" s="28">
         <v>1</v>
@@ -5100,28 +5219,27 @@
         <v>2</v>
       </c>
       <c r="F52" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H52" s="25"/>
+      <c r="I52" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="G52" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="H52" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I52" s="25"/>
       <c r="J52" s="25"/>
       <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-    </row>
-    <row r="53" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="41" t="s">
+    </row>
+    <row r="53" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="38" t="s">
         <v>28</v>
       </c>
       <c r="B53" s="28">
         <v>3002</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D53" s="28">
         <v>1</v>
@@ -5130,28 +5248,27 @@
         <v>2</v>
       </c>
       <c r="F53" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H53" s="25"/>
+      <c r="I53" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="G53" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="H53" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I53" s="25"/>
       <c r="J53" s="25"/>
       <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A54" s="41" t="s">
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A54" s="38" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="28">
         <v>3003</v>
       </c>
       <c r="C54" s="28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D54" s="28">
         <v>1</v>
@@ -5160,24 +5277,24 @@
         <v>2</v>
       </c>
       <c r="F54" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G54" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I54" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="G54" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="H54" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A55" s="41" t="s">
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A55" s="38" t="s">
         <v>25</v>
       </c>
       <c r="B55" s="28">
         <v>3004</v>
       </c>
       <c r="C55" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D55" s="28">
         <v>1</v>
@@ -5186,24 +5303,24 @@
         <v>2</v>
       </c>
       <c r="F55" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I55" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="G55" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="H55" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="41" t="s">
+    </row>
+    <row r="56" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="38" t="s">
         <v>32</v>
       </c>
       <c r="B56" s="28">
         <v>3005</v>
       </c>
       <c r="C56" s="28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D56" s="28">
         <v>1</v>
@@ -5212,28 +5329,27 @@
         <v>2</v>
       </c>
       <c r="F56" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G56" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H56" s="25"/>
+      <c r="I56" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="G56" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="H56" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I56" s="25"/>
       <c r="J56" s="25"/>
       <c r="K56" s="25"/>
-      <c r="L56" s="25"/>
-    </row>
-    <row r="57" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="41" t="s">
+    </row>
+    <row r="57" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="38" t="s">
         <v>33</v>
       </c>
       <c r="B57" s="28">
         <v>3006</v>
       </c>
       <c r="C57" s="28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D57" s="28">
         <v>1</v>
@@ -5242,45 +5358,43 @@
         <v>2</v>
       </c>
       <c r="F57" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G57" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H57" s="25"/>
+      <c r="I57" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="G57" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="H57" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I57" s="25"/>
       <c r="J57" s="25"/>
       <c r="K57" s="25"/>
-      <c r="L57" s="25"/>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A58" s="41" t="s">
-        <v>212</v>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A58" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="F58" s="28"/>
-      <c r="I58" s="25"/>
+        <v>210</v>
+      </c>
+      <c r="H58" s="25"/>
+      <c r="I58" s="28"/>
       <c r="J58" s="25"/>
       <c r="K58" s="25"/>
-      <c r="L58" s="25"/>
+      <c r="L58" s="26"/>
       <c r="M58" s="26"/>
       <c r="N58" s="26"/>
       <c r="O58" s="26"/>
-      <c r="P58" s="26"/>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A59" s="41" t="s">
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A59" s="38" t="s">
         <v>60</v>
       </c>
       <c r="B59" s="28">
         <v>4000</v>
       </c>
       <c r="C59" s="28" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D59" s="28">
         <v>2</v>
@@ -5289,32 +5403,31 @@
         <v>2</v>
       </c>
       <c r="F59" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G59" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H59" s="25"/>
+      <c r="I59" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="G59" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="H59" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I59" s="25"/>
       <c r="J59" s="25"/>
       <c r="K59" s="25"/>
-      <c r="L59" s="25"/>
+      <c r="L59" s="26"/>
       <c r="M59" s="26"/>
       <c r="N59" s="26"/>
       <c r="O59" s="26"/>
-      <c r="P59" s="26"/>
-    </row>
-    <row r="60" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="41" t="s">
+    </row>
+    <row r="60" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="38" t="s">
         <v>61</v>
       </c>
       <c r="B60" s="28">
         <v>4001</v>
       </c>
       <c r="C60" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D60" s="28">
         <v>2</v>
@@ -5323,28 +5436,27 @@
         <v>2</v>
       </c>
       <c r="F60" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="G60" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H60" s="25"/>
+      <c r="I60" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="G60" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="H60" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I60" s="25"/>
       <c r="J60" s="25"/>
       <c r="K60" s="25"/>
-      <c r="L60" s="25"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A61" s="41" t="s">
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A61" s="38" t="s">
         <v>54</v>
       </c>
       <c r="B61" s="28">
         <v>4002</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D61" s="28">
         <v>2</v>
@@ -5352,33 +5464,32 @@
       <c r="E61" s="28">
         <v>2</v>
       </c>
-      <c r="F61" s="28" t="s">
+      <c r="F61" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G61" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H61" s="25"/>
+      <c r="I61" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G61" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="H61" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I61" s="25"/>
       <c r="J61" s="25"/>
       <c r="K61" s="25"/>
-      <c r="L61" s="25"/>
+      <c r="L61" s="26"/>
       <c r="M61" s="26"/>
       <c r="N61" s="26"/>
       <c r="O61" s="26"/>
-      <c r="P61" s="26"/>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A62" s="41" t="s">
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A62" s="38" t="s">
         <v>55</v>
       </c>
       <c r="B62" s="28">
         <v>4003</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D62" s="28">
         <v>2</v>
@@ -5386,33 +5497,32 @@
       <c r="E62" s="28">
         <v>2</v>
       </c>
-      <c r="F62" s="28" t="s">
+      <c r="F62" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="G62" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H62" s="25"/>
+      <c r="I62" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G62" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H62" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I62" s="25"/>
       <c r="J62" s="25"/>
       <c r="K62" s="25"/>
-      <c r="L62" s="25"/>
+      <c r="L62" s="26"/>
       <c r="M62" s="26"/>
       <c r="N62" s="26"/>
       <c r="O62" s="26"/>
-      <c r="P62" s="26"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A63" s="41" t="s">
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A63" s="38" t="s">
         <v>56</v>
       </c>
       <c r="B63" s="28">
         <v>4004</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D63" s="28">
         <v>2</v>
@@ -5420,33 +5530,32 @@
       <c r="E63" s="28">
         <v>2</v>
       </c>
-      <c r="F63" s="28" t="s">
+      <c r="F63" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G63" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="H63" s="25"/>
+      <c r="I63" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G63" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="H63" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="I63" s="25"/>
       <c r="J63" s="25"/>
       <c r="K63" s="25"/>
-      <c r="L63" s="25"/>
+      <c r="L63" s="26"/>
       <c r="M63" s="26"/>
       <c r="N63" s="26"/>
       <c r="O63" s="26"/>
-      <c r="P63" s="26"/>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A64" s="41" t="s">
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A64" s="38" t="s">
         <v>44</v>
       </c>
       <c r="B64" s="28">
         <v>4005</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D64" s="28">
         <v>2</v>
@@ -5454,25 +5563,25 @@
       <c r="E64" s="28">
         <v>2</v>
       </c>
-      <c r="F64" s="28" t="s">
+      <c r="F64" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I64" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G64" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="H64" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A65" s="41" t="s">
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A65" s="38" t="s">
         <v>45</v>
       </c>
       <c r="B65" s="28">
         <v>4006</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D65" s="28">
         <v>2</v>
@@ -5480,25 +5589,25 @@
       <c r="E65" s="28">
         <v>2</v>
       </c>
-      <c r="F65" s="28" t="s">
+      <c r="F65" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="G65" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I65" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G65" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="H65" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A66" s="41" t="s">
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A66" s="38" t="s">
         <v>46</v>
       </c>
       <c r="B66" s="28">
         <v>4007</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D66" s="28">
         <v>2</v>
@@ -5506,25 +5615,25 @@
       <c r="E66" s="28">
         <v>2</v>
       </c>
-      <c r="F66" s="28" t="s">
+      <c r="F66" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G66" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I66" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G66" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="H66" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A67" s="41" t="s">
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A67" s="38" t="s">
         <v>47</v>
       </c>
       <c r="B67" s="28">
         <v>4008</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D67" s="28">
         <v>2</v>
@@ -5532,25 +5641,25 @@
       <c r="E67" s="28">
         <v>2</v>
       </c>
-      <c r="F67" s="28" t="s">
+      <c r="F67" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G67" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I67" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G67" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="H67" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A68" s="41" t="s">
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A68" s="38" t="s">
         <v>48</v>
       </c>
       <c r="B68" s="28">
         <v>4009</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D68" s="28">
         <v>2</v>
@@ -5558,25 +5667,25 @@
       <c r="E68" s="28">
         <v>2</v>
       </c>
-      <c r="F68" s="28" t="s">
+      <c r="F68" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G68" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I68" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G68" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H68" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A69" s="41" t="s">
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A69" s="38" t="s">
         <v>49</v>
       </c>
       <c r="B69" s="28">
         <v>4010</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D69" s="28">
         <v>2</v>
@@ -5584,25 +5693,25 @@
       <c r="E69" s="28">
         <v>2</v>
       </c>
-      <c r="F69" s="28" t="s">
+      <c r="F69" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G69" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I69" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G69" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="H69" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A70" s="41" t="s">
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A70" s="38" t="s">
         <v>50</v>
       </c>
       <c r="B70" s="28">
         <v>4011</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D70" s="28">
         <v>2</v>
@@ -5610,25 +5719,25 @@
       <c r="E70" s="28">
         <v>2</v>
       </c>
-      <c r="F70" s="28" t="s">
+      <c r="F70" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G70" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I70" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G70" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="H70" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A71" s="41" t="s">
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A71" s="38" t="s">
         <v>51</v>
       </c>
       <c r="B71" s="28">
         <v>4012</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D71" s="28">
         <v>2</v>
@@ -5636,25 +5745,25 @@
       <c r="E71" s="28">
         <v>2</v>
       </c>
-      <c r="F71" s="28" t="s">
+      <c r="F71" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G71" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I71" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G71" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="H71" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A72" s="41" t="s">
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A72" s="38" t="s">
         <v>52</v>
       </c>
       <c r="B72" s="28">
         <v>4013</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D72" s="28">
         <v>2</v>
@@ -5662,25 +5771,25 @@
       <c r="E72" s="28">
         <v>2</v>
       </c>
-      <c r="F72" s="28" t="s">
+      <c r="F72" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G72" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I72" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G72" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="H72" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A73" s="41" t="s">
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A73" s="38" t="s">
         <v>53</v>
       </c>
       <c r="B73" s="28">
         <v>4014</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D73" s="28">
         <v>2</v>
@@ -5688,33 +5797,33 @@
       <c r="E73" s="28">
         <v>2</v>
       </c>
-      <c r="F73" s="28" t="s">
+      <c r="F73" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G73" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I73" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="G73" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="H73" s="34" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A74" s="41" t="s">
-        <v>212</v>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A74" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A75" s="41" t="s">
-        <v>240</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A75" s="38" t="s">
+        <v>238</v>
       </c>
       <c r="B75" s="28">
         <v>5000</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D75" s="28">
         <v>0</v>
@@ -5723,24 +5832,24 @@
         <v>3</v>
       </c>
       <c r="F75" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="G75" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="I75" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="G75" s="34" t="s">
-        <v>239</v>
-      </c>
-      <c r="H75" s="34" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A76" s="41" t="s">
-        <v>234</v>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A76" s="38" t="s">
+        <v>232</v>
       </c>
       <c r="B76" s="28">
         <v>5001</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D76" s="28">
         <v>0</v>
@@ -5748,25 +5857,25 @@
       <c r="E76" s="28">
         <v>3</v>
       </c>
-      <c r="F76" s="28" t="s">
+      <c r="F76" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G76" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="I76" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G76" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="H76" s="34" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A77" s="41" t="s">
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A77" s="38" t="s">
         <v>84</v>
       </c>
       <c r="B77" s="28">
         <v>5002</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D77" s="28">
         <v>1</v>
@@ -5774,25 +5883,25 @@
       <c r="E77" s="28">
         <v>3</v>
       </c>
-      <c r="F77" s="28" t="s">
+      <c r="F77" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G77" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="I77" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G77" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="H77" s="34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A78" s="41" t="s">
-        <v>128</v>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A78" s="38" t="s">
+        <v>126</v>
       </c>
       <c r="B78" s="28">
         <v>5003</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D78" s="28">
         <v>1</v>
@@ -5800,25 +5909,25 @@
       <c r="E78" s="28">
         <v>3</v>
       </c>
-      <c r="F78" s="28" t="s">
+      <c r="F78" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G78" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="I78" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G78" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="H78" s="34" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A79" s="41" t="s">
-        <v>235</v>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A79" s="38" t="s">
+        <v>233</v>
       </c>
       <c r="B79" s="28">
         <v>5004</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D79" s="28">
         <v>1</v>
@@ -5826,18 +5935,18 @@
       <c r="E79" s="28">
         <v>3</v>
       </c>
-      <c r="F79" s="28" t="s">
+      <c r="F79" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="G79" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="I79" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G79" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="H79" s="34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A80" s="41" t="s">
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A80" s="38" t="s">
         <v>68</v>
       </c>
       <c r="B80" s="28">
@@ -5852,26 +5961,25 @@
       <c r="E80" s="28">
         <v>3</v>
       </c>
-      <c r="F80" s="28" t="s">
+      <c r="F80" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="G80" s="34">
+        <v>10</v>
+      </c>
+      <c r="H80" s="25"/>
+      <c r="I80" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G80" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="H80" s="34">
-        <v>10</v>
-      </c>
-      <c r="I80" s="25"/>
       <c r="J80" s="25"/>
       <c r="K80" s="25"/>
-      <c r="L80" s="25"/>
+      <c r="L80" s="26"/>
       <c r="M80" s="26"/>
       <c r="N80" s="26"/>
       <c r="O80" s="26"/>
-      <c r="P80" s="26"/>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A81" s="41" t="s">
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A81" s="38" t="s">
         <v>69</v>
       </c>
       <c r="B81" s="28">
@@ -5886,50 +5994,48 @@
       <c r="E81" s="28">
         <v>3</v>
       </c>
-      <c r="F81" s="28" t="s">
+      <c r="F81" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="G81" s="34">
+        <v>10</v>
+      </c>
+      <c r="H81" s="25"/>
+      <c r="I81" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G81" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="H81" s="34">
-        <v>10</v>
-      </c>
-      <c r="I81" s="25"/>
       <c r="J81" s="25"/>
       <c r="K81" s="25"/>
-      <c r="L81" s="25"/>
+      <c r="L81" s="26"/>
       <c r="M81" s="26"/>
       <c r="N81" s="26"/>
       <c r="O81" s="26"/>
-      <c r="P81" s="26"/>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A82" s="41" t="s">
-        <v>212</v>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A82" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="B82" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="F82" s="28"/>
-      <c r="I82" s="25"/>
+        <v>210</v>
+      </c>
+      <c r="H82" s="25"/>
+      <c r="I82" s="28"/>
       <c r="J82" s="25"/>
       <c r="K82" s="25"/>
-      <c r="L82" s="25"/>
+      <c r="L82" s="26"/>
       <c r="M82" s="26"/>
       <c r="N82" s="26"/>
       <c r="O82" s="26"/>
-      <c r="P82" s="26"/>
-    </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A83" s="41" t="s">
-        <v>241</v>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A83" s="38" t="s">
+        <v>239</v>
       </c>
       <c r="B83" s="28">
         <v>5900</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D83" s="28">
         <v>0</v>
@@ -5937,25 +6043,25 @@
       <c r="E83" s="28">
         <v>3</v>
       </c>
-      <c r="F83" s="28" t="s">
+      <c r="F83" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="G83" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="I83" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G83" s="34" t="s">
-        <v>242</v>
-      </c>
-      <c r="H83" s="34" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A84" s="41" t="s">
-        <v>246</v>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A84" s="38" t="s">
+        <v>244</v>
       </c>
       <c r="B84" s="28">
         <v>5901</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D84" s="28">
         <v>0</v>
@@ -5963,25 +6069,25 @@
       <c r="E84" s="28">
         <v>3</v>
       </c>
-      <c r="F84" s="28" t="s">
+      <c r="F84" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="G84" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="I84" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G84" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="H84" s="34" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A85" s="41" t="s">
-        <v>247</v>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A85" s="38" t="s">
+        <v>245</v>
       </c>
       <c r="B85" s="28">
         <v>5902</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D85" s="28">
         <v>0</v>
@@ -5989,25 +6095,25 @@
       <c r="E85" s="28">
         <v>3</v>
       </c>
-      <c r="F85" s="28" t="s">
+      <c r="F85" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="G85" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="I85" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G85" s="34" t="s">
-        <v>243</v>
-      </c>
-      <c r="H85" s="34" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A86" s="41" t="s">
-        <v>248</v>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A86" s="38" t="s">
+        <v>246</v>
       </c>
       <c r="B86" s="28">
         <v>5903</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D86" s="28">
         <v>0</v>
@@ -6015,33 +6121,33 @@
       <c r="E86" s="28">
         <v>3</v>
       </c>
-      <c r="F86" s="28" t="s">
+      <c r="F86" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="G86" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="I86" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G86" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="H86" s="34" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A87" s="41" t="s">
-        <v>212</v>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A87" s="38" t="s">
+        <v>210</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A88" s="41" t="s">
-        <v>256</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A88" s="38" t="s">
+        <v>254</v>
       </c>
       <c r="B88" s="28">
         <v>6000</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D88" s="28">
         <v>0</v>
@@ -6050,24 +6156,24 @@
         <v>4</v>
       </c>
       <c r="F88" s="34" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="G88" s="34" t="s">
         <v>264</v>
       </c>
-      <c r="H88" s="34" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A89" s="41" t="s">
-        <v>257</v>
+      <c r="I88" s="34" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A89" s="38" t="s">
+        <v>255</v>
       </c>
       <c r="B89" s="28">
         <v>6001</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D89" s="28">
         <v>0</v>
@@ -6076,24 +6182,24 @@
         <v>4</v>
       </c>
       <c r="F89" s="34" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G89" s="34" t="s">
-        <v>261</v>
-      </c>
-      <c r="H89" s="34" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A90" s="41" t="s">
-        <v>259</v>
+        <v>264</v>
+      </c>
+      <c r="I89" s="34" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A90" s="38" t="s">
+        <v>257</v>
       </c>
       <c r="B90" s="28">
         <v>6002</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D90" s="28">
         <v>0</v>
@@ -6102,40 +6208,38 @@
         <v>4</v>
       </c>
       <c r="F90" s="34" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G90" s="34" t="s">
-        <v>263</v>
-      </c>
-      <c r="H90" s="34" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.4">
+        <v>264</v>
+      </c>
+      <c r="I90" s="34" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A95" s="35"/>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C100" s="26"/>
     </row>
-    <row r="124" spans="9:16" x14ac:dyDescent="0.4">
-      <c r="I124" s="25"/>
+    <row r="124" spans="8:15" x14ac:dyDescent="0.4">
+      <c r="H124" s="25"/>
       <c r="J124" s="25"/>
       <c r="K124" s="25"/>
-      <c r="L124" s="25"/>
+      <c r="L124" s="26"/>
       <c r="M124" s="26"/>
       <c r="N124" s="26"/>
       <c r="O124" s="26"/>
-      <c r="P124" s="26"/>
-    </row>
-    <row r="125" spans="9:16" x14ac:dyDescent="0.4">
-      <c r="I125" s="25"/>
+    </row>
+    <row r="125" spans="8:15" x14ac:dyDescent="0.4">
+      <c r="H125" s="25"/>
       <c r="J125" s="25"/>
       <c r="K125" s="25"/>
-      <c r="L125" s="25"/>
+      <c r="L125" s="26"/>
       <c r="M125" s="26"/>
       <c r="N125" s="26"/>
       <c r="O125" s="26"/>
-      <c r="P125" s="26"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>